<commit_message>
update n.35 + n.04
</commit_message>
<xml_diff>
--- a/1404.xlsx
+++ b/1404.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chaparsar.RRS\1404\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7BE88E-2B50-4C36-9F42-6B8B12DF9C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9D6ED1-48F1-489C-8247-60EE828346F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N.01 صفحه اصلی" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="284">
   <si>
     <t>اکسل مدیریتی ایستگاه تحقیقات برنج شهید شیرودی تنکابن سال 1404</t>
   </si>
@@ -908,6 +908,12 @@
   </si>
   <si>
     <t xml:space="preserve"> پرینت موقت</t>
+  </si>
+  <si>
+    <t>1404/02/08</t>
+  </si>
+  <si>
+    <t>خرید تخم مرغ</t>
   </si>
 </sst>
 </file>
@@ -918,7 +924,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1033,6 +1039,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="B Titr"/>
+      <charset val="178"/>
     </font>
   </fonts>
   <fills count="23">
@@ -1480,11 +1499,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1727,22 +1747,112 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="19" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="20" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="21" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="14" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1793,7 +1903,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1841,114 +1957,25 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="19" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="20" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="21" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="14" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4315,9 +4342,7 @@
   </sheetPr>
   <dimension ref="D2:L8"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView showGridLines="0" rightToLeft="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4330,16 +4355,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4350,7 +4375,7 @@
       <c r="G4" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="151" t="s">
+      <c r="I4" s="97" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4361,7 +4386,7 @@
       <c r="G5" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="152" t="s">
+      <c r="I5" s="98" t="s">
         <v>281</v>
       </c>
     </row>
@@ -4449,11 +4474,11 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="104"/>
-      <c r="I2" s="85"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="138"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -4461,11 +4486,11 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="104"/>
-      <c r="I3" s="85"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="138"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -4474,12 +4499,12 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="139" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="107"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
       <c r="G5" s="5" t="s">
         <v>212</v>
       </c>
@@ -4684,10 +4709,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="85"/>
+      <c r="I2" s="138"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -4703,8 +4728,8 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="85"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="138"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -4717,10 +4742,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="108" t="s">
+      <c r="H4" s="142" t="s">
         <v>215</v>
       </c>
-      <c r="I4" s="109"/>
+      <c r="I4" s="143"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -4749,12 +4774,12 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
       <c r="E7" s="73"/>
       <c r="F7" s="9"/>
       <c r="G7" s="6"/>
@@ -5135,10 +5160,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="85"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -5155,10 +5180,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="84" t="s">
+      <c r="I3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="85"/>
+      <c r="J3" s="138"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -5172,10 +5197,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="108" t="s">
+      <c r="I4" s="142" t="s">
         <v>145</v>
       </c>
-      <c r="J4" s="109"/>
+      <c r="J4" s="143"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -5206,21 +5231,21 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="61"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="110" t="s">
+      <c r="I7" s="144" t="s">
         <v>151</v>
       </c>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
+      <c r="J7" s="144"/>
+      <c r="K7" s="144"/>
       <c r="L7" s="28"/>
     </row>
     <row r="8" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -5592,10 +5617,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="85"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -5612,10 +5637,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="84" t="s">
+      <c r="I3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="85"/>
+      <c r="J3" s="138"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -5629,10 +5654,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="108" t="s">
+      <c r="I4" s="142" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="109"/>
+      <c r="J4" s="143"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -5663,13 +5688,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="60"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
@@ -5995,10 +6020,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="85"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -6015,10 +6040,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="84" t="s">
+      <c r="I3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="85"/>
+      <c r="J3" s="138"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -6032,10 +6057,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="108" t="s">
+      <c r="I4" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="109"/>
+      <c r="J4" s="143"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -6066,13 +6091,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="17"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
@@ -6413,8 +6438,8 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -6433,10 +6458,14 @@
     <col min="13" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="158" t="s">
+        <v>241</v>
+      </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -6450,14 +6479,11 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="85"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -6470,10 +6496,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="84" t="s">
+      <c r="I3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="85"/>
+      <c r="J3" s="138"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -6487,10 +6513,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="108" t="s">
+      <c r="I4" s="142" t="s">
         <v>129</v>
       </c>
-      <c r="J4" s="109"/>
+      <c r="J4" s="143"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -6521,13 +6547,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="49"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
@@ -6593,7 +6619,7 @@
         <v>1974000</v>
       </c>
       <c r="F10" s="39">
-        <f>F9-E10</f>
+        <f>(F9+D10)-E10</f>
         <v>3026000</v>
       </c>
       <c r="G10" s="9"/>
@@ -6614,7 +6640,7 @@
         <v>106000</v>
       </c>
       <c r="F11" s="39">
-        <f>F10-E11</f>
+        <f>(F10+D11)-E11</f>
         <v>2920000</v>
       </c>
       <c r="G11" s="9"/>
@@ -6635,7 +6661,7 @@
         <v>2800000</v>
       </c>
       <c r="F12" s="39">
-        <f>F11-E12</f>
+        <f t="shared" ref="F12:F14" si="0">(F11+D12)-E12</f>
         <v>120000</v>
       </c>
     </row>
@@ -6654,7 +6680,7 @@
         <v>90000</v>
       </c>
       <c r="F13" s="39">
-        <f t="shared" ref="F13:F14" si="0">F12-E13</f>
+        <f t="shared" si="0"/>
         <v>30000</v>
       </c>
     </row>
@@ -6681,21 +6707,39 @@
       <c r="A15" s="39">
         <v>7</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
+      <c r="B15" s="85" t="s">
+        <v>250</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="39">
+        <v>5000000</v>
+      </c>
       <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
+      <c r="F15" s="39">
+        <f>(F14+D15)-E15</f>
+        <v>3970000</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="27" x14ac:dyDescent="0.25">
       <c r="A16" s="39">
         <v>8</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="85" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>283</v>
+      </c>
       <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
+      <c r="E16" s="39">
+        <v>1200000</v>
+      </c>
+      <c r="F16" s="39">
+        <f>(F15+D16)-E16</f>
+        <v>2770000</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="39">
@@ -6825,8 +6869,9 @@
     <mergeCell ref="A7:E7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L2" location="'صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{0E937C88-4427-4DB9-911F-9ECF29C8B6E1}"/>
     <hyperlink ref="I2:J2" location="'زونکن سه - تنخواه'!A1" display="زونکن شماره سه" xr:uid="{0F6CCBB5-3572-4C33-90EB-64EB5F24F7E3}"/>
+    <hyperlink ref="B1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{0E937C88-4427-4DB9-911F-9ECF29C8B6E1}"/>
+    <hyperlink ref="C1" location="'N.04 دفتر روزانه'!A1" display="دفتر روزانه" xr:uid="{996220C2-EF8C-477F-949C-9BA170C46597}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6874,10 +6919,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="85"/>
+      <c r="I2" s="138"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -6893,10 +6938,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="85"/>
+      <c r="I3" s="138"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -6909,10 +6954,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="108" t="s">
+      <c r="H4" s="142" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="109"/>
+      <c r="I4" s="143"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -6927,13 +6972,13 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:14" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
       <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -7105,10 +7150,10 @@
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="85"/>
+      <c r="G2" s="138"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4" t="s">
         <v>10</v>
@@ -7122,10 +7167,10 @@
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="85"/>
+      <c r="G3" s="138"/>
       <c r="H3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -7136,10 +7181,10 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="F4" s="108" t="s">
+      <c r="F4" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="109"/>
+      <c r="G4" s="143"/>
       <c r="H4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -7152,11 +7197,11 @@
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:12" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="102"/>
       <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:12" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -7233,10 +7278,10 @@
       <c r="C12" s="22"/>
     </row>
     <row r="13" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="111" t="s">
+      <c r="A13" s="145" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="112"/>
+      <c r="B13" s="146"/>
       <c r="C13" s="24">
         <f>SUM(C9:C12)</f>
         <v>0</v>
@@ -7301,10 +7346,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="85"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -7321,10 +7366,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="84" t="s">
+      <c r="I3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="85"/>
+      <c r="J3" s="138"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -7338,10 +7383,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="108" t="s">
+      <c r="I4" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="109"/>
+      <c r="J4" s="143"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -7372,13 +7417,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="27"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
@@ -7714,10 +7759,10 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
-      <c r="L2" s="84" t="s">
+      <c r="L2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="85"/>
+      <c r="M2" s="138"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4" t="s">
         <v>10</v>
@@ -7737,10 +7782,10 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
-      <c r="L3" s="84" t="s">
+      <c r="L3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="85"/>
+      <c r="M3" s="138"/>
       <c r="N3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -7757,10 +7802,10 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="L4" s="108" t="s">
+      <c r="L4" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="109"/>
+      <c r="M4" s="143"/>
       <c r="N4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -7777,10 +7822,10 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="L5" s="113" t="s">
+      <c r="L5" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="114"/>
+      <c r="M5" s="148"/>
       <c r="N5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -7799,16 +7844,16 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:18" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
       <c r="I7" s="74" t="s">
         <v>207</v>
       </c>
@@ -8211,7 +8256,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="96" t="s">
         <v>10</v>
       </c>
     </row>
@@ -8229,16 +8274,16 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
     </row>
     <row r="4" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="53" t="s">
@@ -8265,7 +8310,7 @@
       <c r="I4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="150" t="s">
+      <c r="K4" s="96" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -8285,7 +8330,7 @@
       <c r="I5" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="K5" s="151" t="s">
+      <c r="K5" s="97" t="s">
         <v>232</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -8296,7 +8341,7 @@
       <c r="E6" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="K6" s="152" t="s">
+      <c r="K6" s="98" t="s">
         <v>278</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -8399,10 +8444,10 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="85"/>
+      <c r="L2" s="138"/>
       <c r="M2" s="3"/>
       <c r="N2" s="4" t="s">
         <v>10</v>
@@ -8421,10 +8466,10 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="K3" s="84" t="s">
+      <c r="K3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="85"/>
+      <c r="L3" s="138"/>
       <c r="M3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
@@ -8440,10 +8485,10 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="K4" s="108" t="s">
+      <c r="K4" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="109"/>
+      <c r="L4" s="143"/>
       <c r="M4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -8459,10 +8504,10 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="K5" s="113" t="s">
+      <c r="K5" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="114"/>
+      <c r="L5" s="148"/>
       <c r="M5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -8480,16 +8525,16 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:17" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:17" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -8870,10 +8915,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="85"/>
+      <c r="I2" s="138"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -8889,10 +8934,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="85"/>
+      <c r="I3" s="138"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -8905,10 +8950,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="108" t="s">
+      <c r="H4" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="109"/>
+      <c r="I4" s="143"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -8921,10 +8966,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="113" t="s">
+      <c r="H5" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="114"/>
+      <c r="I5" s="148"/>
       <c r="J5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -8939,13 +8984,13 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -9189,13 +9234,13 @@
       <c r="E29" s="16"/>
     </row>
     <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A41" s="87" t="s">
+      <c r="A41" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="87"/>
-      <c r="C41" s="87"/>
-      <c r="D41" s="87"/>
-      <c r="E41" s="87"/>
+      <c r="B41" s="101"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="101"/>
+      <c r="E41" s="101"/>
     </row>
     <row r="42" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
@@ -9475,10 +9520,10 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="85"/>
+      <c r="K2" s="138"/>
       <c r="L2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -9493,10 +9538,10 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="85"/>
+      <c r="K3" s="138"/>
       <c r="L3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -9511,10 +9556,10 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="J4" s="108" t="s">
+      <c r="J4" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="109"/>
+      <c r="K4" s="143"/>
       <c r="L4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -9529,10 +9574,10 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="J5" s="113" t="s">
+      <c r="J5" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="114"/>
+      <c r="K5" s="148"/>
       <c r="L5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -9549,15 +9594,15 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:16" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -9904,10 +9949,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="85"/>
+      <c r="I2" s="138"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -9920,10 +9965,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="85"/>
+      <c r="I3" s="138"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -9936,10 +9981,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="113" t="s">
+      <c r="H4" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="114"/>
+      <c r="I4" s="148"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -9952,10 +9997,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="108" t="s">
+      <c r="H5" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="109"/>
+      <c r="I5" s="143"/>
       <c r="J5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -9979,13 +10024,13 @@
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -10322,10 +10367,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="115" t="s">
+      <c r="K2" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="116"/>
+      <c r="L2" s="150"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -10415,10 +10460,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="92" t="s">
+      <c r="H2" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="93"/>
+      <c r="I2" s="125"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -10431,10 +10476,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="115" t="s">
+      <c r="H3" s="149" t="s">
         <v>165</v>
       </c>
-      <c r="I3" s="116"/>
+      <c r="I3" s="150"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -10449,13 +10494,13 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -10813,10 +10858,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="92" t="s">
+      <c r="H2" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="93"/>
+      <c r="I2" s="125"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -10828,10 +10873,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="115" t="s">
+      <c r="H3" s="149" t="s">
         <v>175</v>
       </c>
-      <c r="I3" s="116"/>
+      <c r="I3" s="150"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -10845,20 +10890,20 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="27" x14ac:dyDescent="0.25">
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="152" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="152"/>
     </row>
     <row r="6" spans="1:14" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="119" t="s">
+      <c r="A6" s="153" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="72"/>
       <c r="F6" s="72"/>
       <c r="G6" s="72"/>
@@ -10904,11 +10949,11 @@
       <c r="J9"/>
     </row>
     <row r="10" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="117" t="s">
+      <c r="B10" s="151" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="117"/>
-      <c r="D10" s="117"/>
+      <c r="C10" s="151"/>
+      <c r="D10" s="151"/>
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="71"/>
@@ -11057,11 +11102,11 @@
       <c r="J20" s="72"/>
     </row>
     <row r="21" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="117" t="s">
+      <c r="B21" s="151" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
+      <c r="C21" s="151"/>
+      <c r="D21" s="151"/>
       <c r="E21" s="72"/>
       <c r="F21" s="72"/>
       <c r="G21" s="72"/>
@@ -11103,20 +11148,20 @@
       <c r="J24" s="68"/>
     </row>
     <row r="25" spans="1:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="B25" s="118" t="s">
+      <c r="B25" s="152" t="s">
         <v>199</v>
       </c>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
+      <c r="C25" s="152"/>
+      <c r="D25" s="152"/>
+      <c r="E25" s="152"/>
     </row>
     <row r="26" spans="1:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="A26" s="119" t="s">
+      <c r="A26" s="153" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="119"/>
-      <c r="C26" s="119"/>
-      <c r="D26" s="119"/>
+      <c r="B26" s="153"/>
+      <c r="C26" s="153"/>
+      <c r="D26" s="153"/>
     </row>
     <row r="27" spans="1:10" ht="27" x14ac:dyDescent="0.25">
       <c r="B27"/>
@@ -11140,11 +11185,11 @@
       <c r="D29"/>
     </row>
     <row r="30" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="117" t="s">
+      <c r="B30" s="151" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="117"/>
-      <c r="D30" s="117"/>
+      <c r="C30" s="151"/>
+      <c r="D30" s="151"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:10" ht="27" x14ac:dyDescent="0.55000000000000004">
@@ -11238,11 +11283,11 @@
       <c r="D40" s="72"/>
     </row>
     <row r="41" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="117" t="s">
+      <c r="B41" s="151" t="s">
         <v>188</v>
       </c>
-      <c r="C41" s="117"/>
-      <c r="D41" s="117"/>
+      <c r="C41" s="151"/>
+      <c r="D41" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -11305,10 +11350,10 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="93"/>
+      <c r="H2" s="125"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4" t="s">
         <v>10</v>
@@ -11323,10 +11368,10 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="G3" s="115" t="s">
+      <c r="G3" s="149" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="116"/>
+      <c r="H3" s="150"/>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -11340,12 +11385,12 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="101" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -11657,18 +11702,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="7" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="96" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
     </row>
     <row r="4" spans="1:6" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -11714,13 +11759,13 @@
     </row>
     <row r="7" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="101" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
       <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12095,8 +12140,8 @@
       <c r="A122" s="20"/>
     </row>
     <row r="125" spans="1:2" ht="27" x14ac:dyDescent="0.25">
-      <c r="A125" s="87"/>
-      <c r="B125" s="87"/>
+      <c r="A125" s="101"/>
+      <c r="B125" s="101"/>
     </row>
     <row r="126" spans="1:2" ht="27" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
@@ -12208,107 +12253,107 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="126" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="126" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="126" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" style="127" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" style="127" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="127" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="87" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="87" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="88" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="88" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="88" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="89" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="89" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="89" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="45" customWidth="1"/>
     <col min="13" max="13" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="128" t="s">
+      <c r="B1" s="117"/>
+      <c r="C1" s="115" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
     </row>
     <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="131" t="s">
+      <c r="C2" s="103" t="s">
         <v>269</v>
       </c>
-      <c r="D2" s="132"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134" t="s">
+      <c r="D2" s="104"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="154" t="s">
         <v>270</v>
       </c>
-      <c r="G2" s="135"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="137" t="s">
+      <c r="G2" s="155"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="J2" s="138"/>
-      <c r="K2" s="139"/>
-      <c r="L2" s="140" t="s">
+      <c r="J2" s="107"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="141" t="s">
+      <c r="M2" s="90" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="142"/>
-      <c r="B3" s="143"/>
-      <c r="C3" s="144" t="s">
+      <c r="A3" s="112"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="91" t="s">
         <v>272</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="146" t="s">
+      <c r="F3" s="93" t="s">
         <v>272</v>
       </c>
-      <c r="G3" s="146" t="s">
+      <c r="G3" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="H3" s="147" t="s">
+      <c r="H3" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="148" t="s">
+      <c r="I3" s="95" t="s">
         <v>272</v>
       </c>
-      <c r="J3" s="148" t="s">
+      <c r="J3" s="95" t="s">
         <v>273</v>
       </c>
-      <c r="K3" s="148" t="s">
+      <c r="K3" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="149"/>
-      <c r="M3" s="141" t="s">
+      <c r="L3" s="114"/>
+      <c r="M3" s="90" t="s">
         <v>276</v>
       </c>
     </row>
@@ -12316,56 +12361,56 @@
       <c r="A4" s="39">
         <v>1</v>
       </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="121">
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="83">
         <v>0</v>
       </c>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121">
+      <c r="G4" s="83"/>
+      <c r="H4" s="83">
         <f>F4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="122">
+      <c r="I4" s="84">
         <v>0</v>
       </c>
-      <c r="J4" s="122"/>
-      <c r="K4" s="122">
+      <c r="J4" s="84"/>
+      <c r="K4" s="84">
         <f>I4</f>
         <v>0</v>
       </c>
-      <c r="L4" s="123"/>
-      <c r="M4" s="123"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
     </row>
     <row r="5" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
         <v>2</v>
       </c>
-      <c r="B5" s="123" t="s">
+      <c r="B5" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="121"/>
-      <c r="H5" s="121">
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83">
         <f>(H4+F5)-G5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="122"/>
-      <c r="J5" s="122">
+      <c r="I5" s="84"/>
+      <c r="J5" s="84">
         <v>3000000</v>
       </c>
-      <c r="K5" s="122">
+      <c r="K5" s="84">
         <f>(K4+I5)-J5</f>
         <v>-3000000</v>
       </c>
-      <c r="L5" s="124" t="s">
+      <c r="L5" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="M5" s="123" t="s">
+      <c r="M5" s="85" t="s">
         <v>224</v>
       </c>
     </row>
@@ -12373,30 +12418,30 @@
       <c r="A6" s="39">
         <v>3</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="120"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121">
-        <f t="shared" ref="H6:H25" si="0">(H5+F6)-G6</f>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83">
+        <f t="shared" ref="H6:H27" si="0">(H5+F6)-G6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="122"/>
-      <c r="J6" s="122">
+      <c r="I6" s="84"/>
+      <c r="J6" s="84">
         <v>15500000</v>
       </c>
-      <c r="K6" s="122">
+      <c r="K6" s="84">
         <f t="shared" ref="K6:K23" si="1">(K5+I6)-J6</f>
         <v>-18500000</v>
       </c>
-      <c r="L6" s="123" t="s">
+      <c r="L6" s="85" t="s">
         <v>222</v>
       </c>
-      <c r="M6" s="123" t="s">
+      <c r="M6" s="85" t="s">
         <v>224</v>
       </c>
     </row>
@@ -12404,30 +12449,30 @@
       <c r="A7" s="39">
         <v>4</v>
       </c>
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="120"/>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121">
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="122">
+      <c r="I7" s="84">
         <v>15500000</v>
       </c>
-      <c r="J7" s="122"/>
-      <c r="K7" s="122">
+      <c r="J7" s="84"/>
+      <c r="K7" s="84">
         <f t="shared" si="1"/>
         <v>-3000000</v>
       </c>
-      <c r="L7" s="123" t="s">
+      <c r="L7" s="85" t="s">
         <v>226</v>
       </c>
-      <c r="M7" s="123" t="s">
+      <c r="M7" s="85" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12435,30 +12480,30 @@
       <c r="A8" s="39">
         <v>5</v>
       </c>
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121">
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="122">
+      <c r="I8" s="84">
         <v>10000000</v>
       </c>
-      <c r="J8" s="122"/>
-      <c r="K8" s="122">
+      <c r="J8" s="84"/>
+      <c r="K8" s="84">
         <f t="shared" si="1"/>
         <v>7000000</v>
       </c>
-      <c r="L8" s="123" t="s">
+      <c r="L8" s="85" t="s">
         <v>220</v>
       </c>
-      <c r="M8" s="123" t="s">
+      <c r="M8" s="85" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12466,30 +12511,30 @@
       <c r="A9" s="39">
         <v>6</v>
       </c>
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="120"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="121"/>
-      <c r="G9" s="121"/>
-      <c r="H9" s="121">
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="122"/>
-      <c r="J9" s="122">
+      <c r="I9" s="84"/>
+      <c r="J9" s="84">
         <v>1899000</v>
       </c>
-      <c r="K9" s="122">
+      <c r="K9" s="84">
         <f t="shared" si="1"/>
         <v>5101000</v>
       </c>
-      <c r="L9" s="123" t="s">
+      <c r="L9" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="M9" s="123" t="s">
+      <c r="M9" s="85" t="s">
         <v>274</v>
       </c>
     </row>
@@ -12497,88 +12542,88 @@
       <c r="A10" s="39">
         <v>7</v>
       </c>
-      <c r="B10" s="123" t="s">
+      <c r="B10" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="121">
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="122"/>
-      <c r="J10" s="122">
+      <c r="I10" s="84"/>
+      <c r="J10" s="84">
         <v>352000</v>
       </c>
-      <c r="K10" s="122">
+      <c r="K10" s="84">
         <f t="shared" si="1"/>
         <v>4749000</v>
       </c>
-      <c r="L10" s="123" t="s">
+      <c r="L10" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="M10" s="123"/>
+      <c r="M10" s="85"/>
     </row>
     <row r="11" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>8</v>
       </c>
-      <c r="B11" s="123" t="s">
+      <c r="B11" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="121"/>
-      <c r="G11" s="121"/>
-      <c r="H11" s="121">
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="122"/>
-      <c r="J11" s="122">
+      <c r="I11" s="84"/>
+      <c r="J11" s="84">
         <v>3352000</v>
       </c>
-      <c r="K11" s="122">
+      <c r="K11" s="84">
         <f t="shared" si="1"/>
         <v>1397000</v>
       </c>
-      <c r="L11" s="123" t="s">
+      <c r="L11" s="85" t="s">
         <v>124</v>
       </c>
-      <c r="M11" s="123"/>
+      <c r="M11" s="85"/>
     </row>
     <row r="12" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
         <v>9</v>
       </c>
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="121">
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="83">
         <v>5000000</v>
       </c>
-      <c r="G12" s="121"/>
-      <c r="H12" s="121">
+      <c r="G12" s="83"/>
+      <c r="H12" s="83">
         <f t="shared" si="0"/>
         <v>5000000</v>
       </c>
-      <c r="I12" s="122"/>
-      <c r="J12" s="122"/>
-      <c r="K12" s="122">
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="84">
         <f t="shared" si="1"/>
         <v>1397000</v>
       </c>
-      <c r="L12" s="123" t="s">
+      <c r="L12" s="85" t="s">
         <v>220</v>
       </c>
-      <c r="M12" s="123" t="s">
+      <c r="M12" s="85" t="s">
         <v>225</v>
       </c>
     </row>
@@ -12586,117 +12631,117 @@
       <c r="A13" s="39">
         <v>10</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121">
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83">
         <v>1974000</v>
       </c>
-      <c r="H13" s="121">
+      <c r="H13" s="83">
         <f t="shared" si="0"/>
         <v>3026000</v>
       </c>
-      <c r="I13" s="122"/>
-      <c r="J13" s="122"/>
-      <c r="K13" s="122">
+      <c r="I13" s="84"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="84">
         <f t="shared" si="1"/>
         <v>1397000</v>
       </c>
-      <c r="L13" s="123" t="s">
+      <c r="L13" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="M13" s="123"/>
+      <c r="M13" s="85"/>
     </row>
     <row r="14" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
         <v>11</v>
       </c>
-      <c r="B14" s="123" t="s">
+      <c r="B14" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="121"/>
-      <c r="G14" s="121">
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83">
         <v>106000</v>
       </c>
-      <c r="H14" s="121">
+      <c r="H14" s="83">
         <f t="shared" si="0"/>
         <v>2920000</v>
       </c>
-      <c r="I14" s="122"/>
-      <c r="J14" s="122"/>
-      <c r="K14" s="122">
+      <c r="I14" s="84"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="84">
         <f t="shared" si="1"/>
         <v>1397000</v>
       </c>
-      <c r="L14" s="123" t="s">
+      <c r="L14" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="M14" s="123"/>
+      <c r="M14" s="85"/>
     </row>
     <row r="15" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
         <v>12</v>
       </c>
-      <c r="B15" s="123" t="s">
+      <c r="B15" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="121"/>
-      <c r="G15" s="121">
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83">
         <v>2800000</v>
       </c>
-      <c r="H15" s="121">
+      <c r="H15" s="83">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="I15" s="122"/>
-      <c r="J15" s="122"/>
-      <c r="K15" s="122">
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84">
         <f t="shared" si="1"/>
         <v>1397000</v>
       </c>
-      <c r="L15" s="123" t="s">
+      <c r="L15" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="M15" s="123"/>
+      <c r="M15" s="85"/>
     </row>
     <row r="16" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A16" s="39">
         <v>13</v>
       </c>
-      <c r="B16" s="123" t="s">
+      <c r="B16" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="121"/>
-      <c r="G16" s="121"/>
-      <c r="H16" s="121">
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="83">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="I16" s="122"/>
-      <c r="J16" s="122">
+      <c r="I16" s="84"/>
+      <c r="J16" s="84">
         <v>6100000</v>
       </c>
-      <c r="K16" s="122">
+      <c r="K16" s="84">
         <f t="shared" si="1"/>
         <v>-4703000</v>
       </c>
-      <c r="L16" s="123" t="s">
+      <c r="L16" s="85" t="s">
         <v>227</v>
       </c>
-      <c r="M16" s="123" t="s">
+      <c r="M16" s="85" t="s">
         <v>224</v>
       </c>
     </row>
@@ -12704,59 +12749,59 @@
       <c r="A17" s="39">
         <v>14</v>
       </c>
-      <c r="B17" s="123" t="s">
+      <c r="B17" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
-      <c r="H17" s="121">
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="83">
         <f>(H16+F17)-G17</f>
         <v>120000</v>
       </c>
-      <c r="I17" s="122"/>
-      <c r="J17" s="122">
+      <c r="I17" s="84"/>
+      <c r="J17" s="84">
         <v>1000000</v>
       </c>
-      <c r="K17" s="122">
+      <c r="K17" s="84">
         <f t="shared" si="1"/>
         <v>-5703000</v>
       </c>
-      <c r="L17" s="123" t="s">
+      <c r="L17" s="85" t="s">
         <v>211</v>
       </c>
-      <c r="M17" s="123"/>
+      <c r="M17" s="85"/>
     </row>
     <row r="18" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A18" s="39">
         <v>15</v>
       </c>
-      <c r="B18" s="123" t="s">
+      <c r="B18" s="85" t="s">
         <v>210</v>
       </c>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="121"/>
-      <c r="G18" s="121"/>
-      <c r="H18" s="121">
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="83">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="I18" s="122"/>
-      <c r="J18" s="122">
+      <c r="I18" s="84"/>
+      <c r="J18" s="84">
         <v>15000000</v>
       </c>
-      <c r="K18" s="122">
+      <c r="K18" s="84">
         <f t="shared" si="1"/>
         <v>-20703000</v>
       </c>
-      <c r="L18" s="123" t="s">
+      <c r="L18" s="85" t="s">
         <v>228</v>
       </c>
-      <c r="M18" s="123" t="s">
+      <c r="M18" s="85" t="s">
         <v>229</v>
       </c>
     </row>
@@ -12764,30 +12809,30 @@
       <c r="A19" s="39">
         <v>16</v>
       </c>
-      <c r="B19" s="123" t="s">
+      <c r="B19" s="85" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="121"/>
-      <c r="H19" s="121">
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="83">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="I19" s="122">
+      <c r="I19" s="84">
         <v>21100000</v>
       </c>
-      <c r="J19" s="122"/>
-      <c r="K19" s="122">
+      <c r="J19" s="84"/>
+      <c r="K19" s="84">
         <f t="shared" si="1"/>
         <v>397000</v>
       </c>
-      <c r="L19" s="123" t="s">
+      <c r="L19" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="M19" s="123" t="s">
+      <c r="M19" s="85" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12795,523 +12840,544 @@
       <c r="A20" s="39">
         <v>17</v>
       </c>
-      <c r="B20" s="123" t="s">
+      <c r="B20" s="85" t="s">
         <v>250</v>
       </c>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="121">
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="83">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="I20" s="122"/>
-      <c r="J20" s="122">
+      <c r="I20" s="84"/>
+      <c r="J20" s="84">
         <v>2960000</v>
       </c>
-      <c r="K20" s="122">
+      <c r="K20" s="84">
         <f t="shared" si="1"/>
         <v>-2563000</v>
       </c>
-      <c r="L20" s="123" t="s">
+      <c r="L20" s="85" t="s">
         <v>264</v>
       </c>
-      <c r="M20" s="123"/>
+      <c r="M20" s="85"/>
     </row>
     <row r="21" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
         <v>18</v>
       </c>
-      <c r="B21" s="123" t="s">
+      <c r="B21" s="85" t="s">
         <v>250</v>
       </c>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="121"/>
-      <c r="G21" s="121"/>
-      <c r="H21" s="121">
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="I21" s="122"/>
-      <c r="J21" s="122">
+      <c r="I21" s="84"/>
+      <c r="J21" s="84">
         <v>334000</v>
       </c>
-      <c r="K21" s="122">
+      <c r="K21" s="84">
         <f t="shared" si="1"/>
         <v>-2897000</v>
       </c>
-      <c r="L21" s="123" t="s">
+      <c r="L21" s="85" t="s">
         <v>265</v>
       </c>
-      <c r="M21" s="123"/>
+      <c r="M21" s="85"/>
     </row>
     <row r="22" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
         <v>19</v>
       </c>
-      <c r="B22" s="123" t="s">
+      <c r="B22" s="85" t="s">
         <v>250</v>
       </c>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="121"/>
-      <c r="G22" s="121"/>
-      <c r="H22" s="121">
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="I22" s="122"/>
-      <c r="J22" s="122">
+      <c r="I22" s="84"/>
+      <c r="J22" s="84">
         <v>334000</v>
       </c>
-      <c r="K22" s="122">
+      <c r="K22" s="84">
         <f t="shared" si="1"/>
         <v>-3231000</v>
       </c>
-      <c r="L22" s="123" t="s">
+      <c r="L22" s="85" t="s">
         <v>265</v>
       </c>
-      <c r="M22" s="123"/>
+      <c r="M22" s="85"/>
     </row>
     <row r="23" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A23" s="39">
         <v>20</v>
       </c>
-      <c r="B23" s="123" t="s">
+      <c r="B23" s="85" t="s">
         <v>250</v>
       </c>
-      <c r="C23" s="120"/>
-      <c r="D23" s="120"/>
-      <c r="E23" s="120"/>
-      <c r="F23" s="121"/>
-      <c r="G23" s="121"/>
-      <c r="H23" s="121">
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="83">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="I23" s="122"/>
-      <c r="J23" s="122">
+      <c r="I23" s="84"/>
+      <c r="J23" s="84">
         <v>334000</v>
       </c>
-      <c r="K23" s="122">
+      <c r="K23" s="84">
         <f t="shared" si="1"/>
         <v>-3565000</v>
       </c>
-      <c r="L23" s="123" t="s">
+      <c r="L23" s="85" t="s">
         <v>265</v>
       </c>
-      <c r="M23" s="123"/>
+      <c r="M23" s="85"/>
     </row>
     <row r="24" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A24" s="39">
         <v>22</v>
       </c>
-      <c r="B24" s="123" t="s">
+      <c r="B24" s="85" t="s">
         <v>250</v>
       </c>
-      <c r="C24" s="120"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="120"/>
-      <c r="F24" s="121"/>
-      <c r="G24" s="121">
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83">
         <v>90000</v>
       </c>
-      <c r="H24" s="121">
+      <c r="H24" s="83">
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-      <c r="I24" s="122"/>
-      <c r="J24" s="122"/>
-      <c r="K24" s="122"/>
-      <c r="L24" s="123" t="s">
+      <c r="I24" s="84"/>
+      <c r="J24" s="84"/>
+      <c r="K24" s="84"/>
+      <c r="L24" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="M24" s="123"/>
+      <c r="M24" s="85"/>
     </row>
     <row r="25" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A25" s="39">
         <v>23</v>
       </c>
-      <c r="B25" s="123" t="s">
+      <c r="B25" s="85" t="s">
         <v>250</v>
       </c>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="121"/>
-      <c r="G25" s="121">
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83">
         <v>1060000</v>
       </c>
-      <c r="H25" s="121">
+      <c r="H25" s="83">
         <f t="shared" si="0"/>
         <v>-1030000</v>
       </c>
-      <c r="I25" s="122"/>
-      <c r="J25" s="122"/>
-      <c r="K25" s="122"/>
-      <c r="L25" s="123" t="s">
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="85" t="s">
         <v>268</v>
       </c>
-      <c r="M25" s="123"/>
+      <c r="M25" s="85"/>
     </row>
     <row r="26" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
         <v>24</v>
       </c>
-      <c r="B26" s="123"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="120"/>
-      <c r="F26" s="121"/>
-      <c r="G26" s="121"/>
-      <c r="H26" s="121"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="122"/>
-      <c r="K26" s="122"/>
-      <c r="L26" s="123"/>
-      <c r="M26" s="123"/>
+      <c r="B26" s="85" t="s">
+        <v>250</v>
+      </c>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="83">
+        <v>5000000</v>
+      </c>
+      <c r="G26" s="83"/>
+      <c r="H26" s="83">
+        <f t="shared" si="0"/>
+        <v>3970000</v>
+      </c>
+      <c r="I26" s="84"/>
+      <c r="J26" s="84"/>
+      <c r="K26" s="84"/>
+      <c r="L26" s="85" t="s">
+        <v>131</v>
+      </c>
+      <c r="M26" s="85" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
         <v>25</v>
       </c>
-      <c r="B27" s="123"/>
-      <c r="C27" s="120"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="120"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="122"/>
-      <c r="J27" s="122"/>
-      <c r="K27" s="122"/>
-      <c r="L27" s="123"/>
-      <c r="M27" s="123"/>
+      <c r="B27" s="85" t="s">
+        <v>282</v>
+      </c>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="83">
+        <v>1200000</v>
+      </c>
+      <c r="H27" s="83">
+        <f t="shared" si="0"/>
+        <v>2770000</v>
+      </c>
+      <c r="I27" s="84"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="84"/>
+      <c r="L27" s="85" t="s">
+        <v>283</v>
+      </c>
+      <c r="M27" s="85"/>
     </row>
     <row r="28" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
         <v>26</v>
       </c>
-      <c r="B28" s="123"/>
-      <c r="C28" s="120"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="120"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="121"/>
-      <c r="I28" s="122"/>
-      <c r="J28" s="122"/>
-      <c r="K28" s="122"/>
-      <c r="L28" s="123"/>
-      <c r="M28" s="123"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="84"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="85"/>
     </row>
     <row r="29" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
         <v>27</v>
       </c>
-      <c r="B29" s="123"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="120"/>
-      <c r="E29" s="120"/>
-      <c r="F29" s="121"/>
-      <c r="G29" s="121"/>
-      <c r="H29" s="121"/>
-      <c r="I29" s="122"/>
-      <c r="J29" s="122"/>
-      <c r="K29" s="122"/>
-      <c r="L29" s="123"/>
-      <c r="M29" s="123"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="83"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="84"/>
+      <c r="K29" s="84"/>
+      <c r="L29" s="85"/>
+      <c r="M29" s="85"/>
     </row>
     <row r="30" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A30" s="39">
         <v>28</v>
       </c>
-      <c r="B30" s="123"/>
-      <c r="C30" s="120"/>
-      <c r="D30" s="120"/>
-      <c r="E30" s="120"/>
-      <c r="F30" s="121"/>
-      <c r="G30" s="121"/>
-      <c r="H30" s="121"/>
-      <c r="I30" s="122"/>
-      <c r="J30" s="122"/>
-      <c r="K30" s="122"/>
-      <c r="L30" s="123"/>
-      <c r="M30" s="123"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="84"/>
+      <c r="K30" s="84"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="85"/>
     </row>
     <row r="31" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
         <v>29</v>
       </c>
-      <c r="B31" s="123"/>
-      <c r="C31" s="120"/>
-      <c r="D31" s="120"/>
-      <c r="E31" s="120"/>
-      <c r="F31" s="121"/>
-      <c r="G31" s="121"/>
-      <c r="H31" s="121"/>
-      <c r="I31" s="122"/>
-      <c r="J31" s="122"/>
-      <c r="K31" s="122"/>
-      <c r="L31" s="123"/>
-      <c r="M31" s="123"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="84"/>
+      <c r="J31" s="84"/>
+      <c r="K31" s="84"/>
+      <c r="L31" s="85"/>
+      <c r="M31" s="85"/>
     </row>
     <row r="32" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A32" s="39">
         <v>30</v>
       </c>
-      <c r="B32" s="123"/>
-      <c r="C32" s="120"/>
-      <c r="D32" s="120"/>
-      <c r="E32" s="120"/>
-      <c r="F32" s="121"/>
-      <c r="G32" s="121"/>
-      <c r="H32" s="121"/>
-      <c r="I32" s="122"/>
-      <c r="J32" s="122"/>
-      <c r="K32" s="122"/>
-      <c r="L32" s="123"/>
-      <c r="M32" s="123"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="84"/>
+      <c r="J32" s="84"/>
+      <c r="K32" s="84"/>
+      <c r="L32" s="85"/>
+      <c r="M32" s="85"/>
     </row>
     <row r="33" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A33" s="39">
         <v>31</v>
       </c>
-      <c r="B33" s="123"/>
-      <c r="C33" s="120"/>
-      <c r="D33" s="120"/>
-      <c r="E33" s="120"/>
-      <c r="F33" s="121"/>
-      <c r="G33" s="121"/>
-      <c r="H33" s="121"/>
-      <c r="I33" s="122"/>
-      <c r="J33" s="122"/>
-      <c r="K33" s="122"/>
-      <c r="L33" s="123"/>
-      <c r="M33" s="123"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="84"/>
+      <c r="K33" s="84"/>
+      <c r="L33" s="85"/>
+      <c r="M33" s="85"/>
     </row>
     <row r="34" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
         <v>32</v>
       </c>
-      <c r="B34" s="123"/>
-      <c r="C34" s="120"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="121"/>
-      <c r="I34" s="122"/>
-      <c r="J34" s="122"/>
-      <c r="K34" s="122"/>
-      <c r="L34" s="123"/>
-      <c r="M34" s="123"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="84"/>
+      <c r="J34" s="84"/>
+      <c r="K34" s="84"/>
+      <c r="L34" s="85"/>
+      <c r="M34" s="85"/>
     </row>
     <row r="35" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A35" s="39">
         <v>33</v>
       </c>
-      <c r="B35" s="123"/>
-      <c r="C35" s="120"/>
-      <c r="D35" s="120"/>
-      <c r="E35" s="120"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="121"/>
-      <c r="H35" s="121"/>
-      <c r="I35" s="122"/>
-      <c r="J35" s="122"/>
-      <c r="K35" s="122"/>
-      <c r="L35" s="123"/>
-      <c r="M35" s="123"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="84"/>
+      <c r="J35" s="84"/>
+      <c r="K35" s="84"/>
+      <c r="L35" s="85"/>
+      <c r="M35" s="85"/>
     </row>
     <row r="36" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
         <v>34</v>
       </c>
-      <c r="B36" s="123"/>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="120"/>
-      <c r="F36" s="121"/>
-      <c r="G36" s="121"/>
-      <c r="H36" s="121"/>
-      <c r="I36" s="122"/>
-      <c r="J36" s="122"/>
-      <c r="K36" s="122"/>
-      <c r="L36" s="123"/>
-      <c r="M36" s="123"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="84"/>
+      <c r="J36" s="84"/>
+      <c r="K36" s="84"/>
+      <c r="L36" s="85"/>
+      <c r="M36" s="85"/>
     </row>
     <row r="37" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A37" s="39">
         <v>35</v>
       </c>
-      <c r="B37" s="123"/>
-      <c r="C37" s="120"/>
-      <c r="D37" s="120"/>
-      <c r="E37" s="120"/>
-      <c r="F37" s="121"/>
-      <c r="G37" s="121"/>
-      <c r="H37" s="121"/>
-      <c r="I37" s="122"/>
-      <c r="J37" s="122"/>
-      <c r="K37" s="122"/>
-      <c r="L37" s="123"/>
-      <c r="M37" s="123"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="84"/>
+      <c r="L37" s="85"/>
+      <c r="M37" s="85"/>
     </row>
     <row r="38" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A38" s="39">
         <v>36</v>
       </c>
-      <c r="B38" s="123"/>
-      <c r="C38" s="120"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="120"/>
-      <c r="F38" s="121"/>
-      <c r="G38" s="121"/>
-      <c r="H38" s="121"/>
-      <c r="I38" s="122"/>
-      <c r="J38" s="122"/>
-      <c r="K38" s="122"/>
-      <c r="L38" s="123"/>
-      <c r="M38" s="123"/>
+      <c r="B38" s="85"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="84"/>
+      <c r="J38" s="84"/>
+      <c r="K38" s="84"/>
+      <c r="L38" s="85"/>
+      <c r="M38" s="85"/>
     </row>
     <row r="39" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A39" s="39">
         <v>37</v>
       </c>
-      <c r="B39" s="123"/>
-      <c r="C39" s="120"/>
-      <c r="D39" s="120"/>
-      <c r="E39" s="120"/>
-      <c r="F39" s="121"/>
-      <c r="G39" s="121"/>
-      <c r="H39" s="121"/>
-      <c r="I39" s="122"/>
-      <c r="J39" s="122"/>
-      <c r="K39" s="122"/>
-      <c r="L39" s="123"/>
-      <c r="M39" s="123"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="84"/>
+      <c r="J39" s="84"/>
+      <c r="K39" s="84"/>
+      <c r="L39" s="85"/>
+      <c r="M39" s="85"/>
     </row>
     <row r="40" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A40" s="39">
         <v>38</v>
       </c>
-      <c r="B40" s="123"/>
-      <c r="C40" s="120"/>
-      <c r="D40" s="120"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="121"/>
-      <c r="G40" s="121"/>
-      <c r="H40" s="121"/>
-      <c r="I40" s="122"/>
-      <c r="J40" s="122"/>
-      <c r="K40" s="122"/>
-      <c r="L40" s="123"/>
-      <c r="M40" s="123"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="84"/>
+      <c r="J40" s="84"/>
+      <c r="K40" s="84"/>
+      <c r="L40" s="85"/>
+      <c r="M40" s="85"/>
     </row>
     <row r="41" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A41" s="39">
         <v>39</v>
       </c>
-      <c r="B41" s="123"/>
-      <c r="C41" s="120"/>
-      <c r="D41" s="120"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="121"/>
-      <c r="G41" s="121"/>
-      <c r="H41" s="121"/>
-      <c r="I41" s="122"/>
-      <c r="J41" s="122"/>
-      <c r="K41" s="122"/>
-      <c r="L41" s="123"/>
-      <c r="M41" s="123"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="82"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="82"/>
+      <c r="F41" s="83"/>
+      <c r="G41" s="83"/>
+      <c r="H41" s="83"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="84"/>
+      <c r="K41" s="84"/>
+      <c r="L41" s="85"/>
+      <c r="M41" s="85"/>
     </row>
     <row r="42" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A42" s="39">
         <v>40</v>
       </c>
-      <c r="B42" s="123"/>
-      <c r="C42" s="120"/>
-      <c r="D42" s="120"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="121"/>
-      <c r="G42" s="121"/>
-      <c r="H42" s="121"/>
-      <c r="I42" s="122"/>
-      <c r="J42" s="122"/>
-      <c r="K42" s="122"/>
-      <c r="L42" s="123"/>
-      <c r="M42" s="123"/>
+      <c r="B42" s="85"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="83"/>
+      <c r="G42" s="83"/>
+      <c r="H42" s="83"/>
+      <c r="I42" s="84"/>
+      <c r="J42" s="84"/>
+      <c r="K42" s="84"/>
+      <c r="L42" s="85"/>
+      <c r="M42" s="85"/>
     </row>
     <row r="43" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A43" s="39">
         <v>41</v>
       </c>
-      <c r="B43" s="123"/>
-      <c r="C43" s="120"/>
-      <c r="D43" s="120"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="121"/>
-      <c r="G43" s="121"/>
-      <c r="H43" s="121"/>
-      <c r="I43" s="122"/>
-      <c r="J43" s="122"/>
-      <c r="K43" s="122"/>
-      <c r="L43" s="123"/>
-      <c r="M43" s="123"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="82"/>
+      <c r="D43" s="82"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
+      <c r="H43" s="83"/>
+      <c r="I43" s="84"/>
+      <c r="J43" s="84"/>
+      <c r="K43" s="84"/>
+      <c r="L43" s="85"/>
+      <c r="M43" s="85"/>
     </row>
     <row r="44" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A44" s="39">
         <v>42</v>
       </c>
-      <c r="B44" s="123"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="121"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="121"/>
-      <c r="I44" s="122"/>
-      <c r="J44" s="122"/>
-      <c r="K44" s="122"/>
-      <c r="L44" s="123"/>
-      <c r="M44" s="123"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="83"/>
+      <c r="H44" s="83"/>
+      <c r="I44" s="84"/>
+      <c r="J44" s="84"/>
+      <c r="K44" s="84"/>
+      <c r="L44" s="85"/>
+      <c r="M44" s="85"/>
     </row>
     <row r="45" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A45" s="39">
         <v>43</v>
       </c>
-      <c r="B45" s="123"/>
-      <c r="C45" s="120"/>
-      <c r="D45" s="120"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="121"/>
-      <c r="G45" s="121"/>
-      <c r="H45" s="121"/>
-      <c r="I45" s="122"/>
-      <c r="J45" s="122"/>
-      <c r="K45" s="122"/>
-      <c r="L45" s="123"/>
-      <c r="M45" s="123"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
+      <c r="H45" s="83"/>
+      <c r="I45" s="84"/>
+      <c r="J45" s="84"/>
+      <c r="K45" s="84"/>
+      <c r="L45" s="85"/>
+      <c r="M45" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{C9A86160-01A7-4FFF-AE85-83614874BA51}"/>
+    <hyperlink ref="F2:H2" location="'N.35 تنخواه پیمانکاری دیوارکشی'!A1" display="تنخواه دیوارکشی آقای سعیدی" xr:uid="{1B951EA9-90AF-4C68-B11E-FE74F818619A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13345,10 +13411,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="156"/>
+      <c r="B1" s="119"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -13361,10 +13427,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="89"/>
+      <c r="I2" s="121"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -13377,10 +13443,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="91"/>
+      <c r="I3" s="123"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -13409,13 +13475,13 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:13" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -13684,13 +13750,13 @@
       <c r="M30" s="6"/>
     </row>
     <row r="33" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A33" s="87" t="s">
+      <c r="A33" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="87"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="101"/>
       <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" ht="27" x14ac:dyDescent="0.25">
@@ -13914,14 +13980,14 @@
       <c r="F54" s="21"/>
     </row>
     <row r="57" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A57" s="86" t="s">
+      <c r="A57" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="86"/>
-      <c r="C57" s="86"/>
-      <c r="D57" s="86"/>
-      <c r="E57" s="86"/>
-      <c r="F57" s="86"/>
+      <c r="B57" s="102"/>
+      <c r="C57" s="102"/>
+      <c r="D57" s="102"/>
+      <c r="E57" s="102"/>
+      <c r="F57" s="102"/>
     </row>
     <row r="58" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
@@ -14143,12 +14209,12 @@
       <c r="F78" s="20"/>
     </row>
     <row r="82" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="B82" s="86"/>
-      <c r="C82" s="86"/>
-      <c r="D82" s="86"/>
+      <c r="B82" s="102"/>
+      <c r="C82" s="102"/>
+      <c r="D82" s="102"/>
     </row>
     <row r="83" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
@@ -14325,15 +14391,15 @@
       <c r="D103" s="22"/>
     </row>
     <row r="106" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A106" s="87" t="s">
+      <c r="A106" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="B106" s="87"/>
-      <c r="C106" s="87"/>
-      <c r="D106" s="87"/>
-      <c r="E106" s="87"/>
-      <c r="F106" s="87"/>
-      <c r="G106" s="87"/>
+      <c r="B106" s="101"/>
+      <c r="C106" s="101"/>
+      <c r="D106" s="101"/>
+      <c r="E106" s="101"/>
+      <c r="F106" s="101"/>
+      <c r="G106" s="101"/>
     </row>
     <row r="107" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
@@ -14583,16 +14649,16 @@
       <c r="G127" s="20"/>
     </row>
     <row r="130" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A130" s="87" t="s">
+      <c r="A130" s="101" t="s">
         <v>110</v>
       </c>
-      <c r="B130" s="87"/>
-      <c r="C130" s="87"/>
-      <c r="D130" s="87"/>
-      <c r="E130" s="87"/>
-      <c r="F130" s="87"/>
-      <c r="G130" s="87"/>
-      <c r="H130" s="87"/>
+      <c r="B130" s="101"/>
+      <c r="C130" s="101"/>
+      <c r="D130" s="101"/>
+      <c r="E130" s="101"/>
+      <c r="F130" s="101"/>
+      <c r="G130" s="101"/>
+      <c r="H130" s="101"/>
     </row>
     <row r="131" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
@@ -14861,13 +14927,13 @@
       <c r="H151" s="10"/>
     </row>
     <row r="155" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A155" s="87" t="s">
+      <c r="A155" s="101" t="s">
         <v>143</v>
       </c>
-      <c r="B155" s="87"/>
-      <c r="C155" s="87"/>
-      <c r="D155" s="87"/>
-      <c r="E155" s="87"/>
+      <c r="B155" s="101"/>
+      <c r="C155" s="101"/>
+      <c r="D155" s="101"/>
+      <c r="E155" s="101"/>
       <c r="F155" s="63"/>
     </row>
     <row r="156" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -15091,13 +15157,13 @@
       <c r="F176" s="39"/>
     </row>
     <row r="179" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A179" s="87" t="s">
+      <c r="A179" s="101" t="s">
         <v>145</v>
       </c>
-      <c r="B179" s="87"/>
-      <c r="C179" s="87"/>
-      <c r="D179" s="87"/>
-      <c r="E179" s="87"/>
+      <c r="B179" s="101"/>
+      <c r="C179" s="101"/>
+      <c r="D179" s="101"/>
+      <c r="E179" s="101"/>
       <c r="F179" s="66"/>
     </row>
     <row r="180" spans="1:6" ht="27" x14ac:dyDescent="0.25">
@@ -15317,14 +15383,14 @@
       <c r="F200" s="39"/>
     </row>
     <row r="204" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A204" s="86" t="s">
+      <c r="A204" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="B204" s="86"/>
-      <c r="C204" s="86"/>
-      <c r="D204" s="86"/>
-      <c r="E204" s="86"/>
-      <c r="F204" s="86"/>
+      <c r="B204" s="102"/>
+      <c r="C204" s="102"/>
+      <c r="D204" s="102"/>
+      <c r="E204" s="102"/>
+      <c r="F204" s="102"/>
     </row>
     <row r="205" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A205" s="78" t="s">
@@ -15845,11 +15911,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A33:E33"/>
     <mergeCell ref="A57:F57"/>
     <mergeCell ref="A204:F204"/>
     <mergeCell ref="A179:E179"/>
@@ -15857,6 +15918,11 @@
     <mergeCell ref="A82:D82"/>
     <mergeCell ref="A106:G106"/>
     <mergeCell ref="A130:H130"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A33:E33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{9E228265-015F-4ED7-804E-491796425E13}"/>
@@ -15890,16 +15956,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="156"/>
+      <c r="B1" s="119"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="92" t="s">
+      <c r="J2" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="93"/>
+      <c r="K2" s="125"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -15939,10 +16005,10 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="92" t="s">
+      <c r="J12" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="93"/>
+      <c r="K12" s="125"/>
     </row>
     <row r="13" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="2">
@@ -16013,7 +16079,7 @@
       </c>
     </row>
     <row r="24" spans="9:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="94" t="s">
+      <c r="I24" s="126" t="s">
         <v>76</v>
       </c>
       <c r="J24" s="2">
@@ -16024,7 +16090,7 @@
       </c>
     </row>
     <row r="25" spans="9:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I25" s="95"/>
+      <c r="I25" s="127"/>
       <c r="J25" s="2" t="s">
         <v>74</v>
       </c>
@@ -16073,10 +16139,10 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="96" t="s">
+      <c r="K2" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="97"/>
+      <c r="L2" s="129"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -16154,10 +16220,10 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="98" t="s">
+      <c r="K2" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="99"/>
+      <c r="L2" s="131"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -16253,10 +16319,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="101"/>
+      <c r="J2" s="133"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -16273,10 +16339,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="100" t="s">
+      <c r="I3" s="132" t="s">
         <v>157</v>
       </c>
-      <c r="J3" s="101"/>
+      <c r="J3" s="133"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -16290,10 +16356,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="102" t="s">
+      <c r="I4" s="134" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="103"/>
+      <c r="J4" s="135"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -16324,13 +16390,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="101" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="61"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>

</xml_diff>

<commit_message>
update n.04 + n.34
</commit_message>
<xml_diff>
--- a/1404.xlsx
+++ b/1404.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chaparsar.RRS\1404\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917B52BB-B46E-4304-B761-159AA9064036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB4D2E9-EFAF-47B5-8E19-7D9BFE4D9E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N.01 صفحه اصلی" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="288">
   <si>
     <t>اکسل مدیریتی ایستگاه تحقیقات برنج شهید شیرودی تنکابن سال 1404</t>
   </si>
@@ -917,6 +917,15 @@
   </si>
   <si>
     <t>تحویل کامل</t>
+  </si>
+  <si>
+    <t>خرید شوینده و سایروسایل</t>
+  </si>
+  <si>
+    <t>خرید شوینده و سایر وسایل</t>
+  </si>
+  <si>
+    <t>فروتن</t>
   </si>
 </sst>
 </file>
@@ -4457,7 +4466,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5591,7 +5600,7 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
+    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -6002,15 +6011,15 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="9" bestFit="1" customWidth="1"/>
@@ -6203,7 +6212,7 @@
         <v>352000</v>
       </c>
       <c r="F11" s="39">
-        <f t="shared" ref="F11:F17" si="0">F10-E11</f>
+        <f t="shared" ref="F11:F18" si="0">F10-E11</f>
         <v>7749000</v>
       </c>
       <c r="G11" s="9"/>
@@ -6327,11 +6336,20 @@
       <c r="A18" s="39">
         <v>10</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
+      <c r="B18" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>285</v>
+      </c>
       <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
+      <c r="E18" s="39">
+        <v>5267000</v>
+      </c>
+      <c r="F18" s="39">
+        <f t="shared" si="0"/>
+        <v>-5832000</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A19" s="39">
@@ -12271,9 +12289,9 @@
   </sheetPr>
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12454,7 +12472,7 @@
         <v>15500000</v>
       </c>
       <c r="K6" s="84">
-        <f t="shared" ref="K6:K23" si="1">(K5+I6)-J6</f>
+        <f t="shared" ref="K6:K28" si="1">(K5+I6)-J6</f>
         <v>-18500000</v>
       </c>
       <c r="L6" s="85" t="s">
@@ -12991,7 +13009,10 @@
       </c>
       <c r="I24" s="84"/>
       <c r="J24" s="84"/>
-      <c r="K24" s="84"/>
+      <c r="K24" s="84">
+        <f t="shared" si="1"/>
+        <v>-3565000</v>
+      </c>
       <c r="L24" s="85" t="s">
         <v>138</v>
       </c>
@@ -13017,7 +13038,10 @@
       </c>
       <c r="I25" s="84"/>
       <c r="J25" s="84"/>
-      <c r="K25" s="84"/>
+      <c r="K25" s="84">
+        <f t="shared" si="1"/>
+        <v>-3565000</v>
+      </c>
       <c r="L25" s="85" t="s">
         <v>267</v>
       </c>
@@ -13043,7 +13067,10 @@
       </c>
       <c r="I26" s="84"/>
       <c r="J26" s="84"/>
-      <c r="K26" s="84"/>
+      <c r="K26" s="84">
+        <f t="shared" si="1"/>
+        <v>-3565000</v>
+      </c>
       <c r="L26" s="85" t="s">
         <v>131</v>
       </c>
@@ -13071,7 +13098,10 @@
       </c>
       <c r="I27" s="84"/>
       <c r="J27" s="84"/>
-      <c r="K27" s="84"/>
+      <c r="K27" s="84">
+        <f t="shared" si="1"/>
+        <v>-3565000</v>
+      </c>
       <c r="L27" s="85" t="s">
         <v>282</v>
       </c>
@@ -13081,7 +13111,9 @@
       <c r="A28" s="39">
         <v>26</v>
       </c>
-      <c r="B28" s="85"/>
+      <c r="B28" s="85" t="s">
+        <v>281</v>
+      </c>
       <c r="C28" s="82"/>
       <c r="D28" s="82"/>
       <c r="E28" s="82"/>
@@ -13089,10 +13121,19 @@
       <c r="G28" s="83"/>
       <c r="H28" s="83"/>
       <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="84"/>
-      <c r="L28" s="85"/>
-      <c r="M28" s="85"/>
+      <c r="J28" s="84">
+        <v>5267000</v>
+      </c>
+      <c r="K28" s="84">
+        <f t="shared" si="1"/>
+        <v>-8832000</v>
+      </c>
+      <c r="L28" s="85" t="s">
+        <v>286</v>
+      </c>
+      <c r="M28" s="85" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
@@ -16302,7 +16343,7 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update n.04 + n.31
</commit_message>
<xml_diff>
--- a/1404.xlsx
+++ b/1404.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chaparsar.RRS\1404\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB4D2E9-EFAF-47B5-8E19-7D9BFE4D9E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5E5FE5-F797-4043-B4FE-C57F897CD77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N.01 صفحه اصلی" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="290">
   <si>
     <t>اکسل مدیریتی ایستگاه تحقیقات برنج شهید شیرودی تنکابن سال 1404</t>
   </si>
@@ -926,6 +926,12 @@
   </si>
   <si>
     <t>فروتن</t>
+  </si>
+  <si>
+    <t>کود اوره مرکبات</t>
+  </si>
+  <si>
+    <t>وفادار</t>
   </si>
 </sst>
 </file>
@@ -4689,8 +4695,8 @@
   </sheetPr>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -4870,12 +4876,24 @@
       <c r="A11" s="39">
         <v>6</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="76"/>
+      <c r="B11" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="D11" s="11">
+        <v>100</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="39">
+        <v>8000000</v>
+      </c>
+      <c r="G11" s="76" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
@@ -12287,11 +12305,11 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+    <sheetView showGridLines="0" rightToLeft="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12472,7 +12490,7 @@
         <v>15500000</v>
       </c>
       <c r="K6" s="84">
-        <f t="shared" ref="K6:K28" si="1">(K5+I6)-J6</f>
+        <f t="shared" ref="K6:K29" si="1">(K5+I6)-J6</f>
         <v>-18500000</v>
       </c>
       <c r="L6" s="85" t="s">
@@ -13108,9 +13126,7 @@
       <c r="M27" s="85"/>
     </row>
     <row r="28" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A28" s="39">
-        <v>26</v>
-      </c>
+      <c r="A28" s="39"/>
       <c r="B28" s="85" t="s">
         <v>281</v>
       </c>
@@ -13122,24 +13138,26 @@
       <c r="H28" s="83"/>
       <c r="I28" s="84"/>
       <c r="J28" s="84">
-        <v>5267000</v>
+        <v>8000000</v>
       </c>
       <c r="K28" s="84">
         <f t="shared" si="1"/>
-        <v>-8832000</v>
+        <v>-11565000</v>
       </c>
       <c r="L28" s="85" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="M28" s="85" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
-        <v>27</v>
-      </c>
-      <c r="B29" s="85"/>
+        <v>26</v>
+      </c>
+      <c r="B29" s="85" t="s">
+        <v>281</v>
+      </c>
       <c r="C29" s="82"/>
       <c r="D29" s="82"/>
       <c r="E29" s="82"/>
@@ -13147,14 +13165,23 @@
       <c r="G29" s="83"/>
       <c r="H29" s="83"/>
       <c r="I29" s="84"/>
-      <c r="J29" s="84"/>
-      <c r="K29" s="84"/>
-      <c r="L29" s="85"/>
-      <c r="M29" s="85"/>
+      <c r="J29" s="84">
+        <v>5267000</v>
+      </c>
+      <c r="K29" s="84">
+        <f t="shared" si="1"/>
+        <v>-16832000</v>
+      </c>
+      <c r="L29" s="85" t="s">
+        <v>286</v>
+      </c>
+      <c r="M29" s="85" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A30" s="39">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="85"/>
       <c r="C30" s="82"/>
@@ -13171,7 +13198,7 @@
     </row>
     <row r="31" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="85"/>
       <c r="C31" s="82"/>
@@ -13188,7 +13215,7 @@
     </row>
     <row r="32" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A32" s="39">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="85"/>
       <c r="C32" s="82"/>
@@ -13205,7 +13232,7 @@
     </row>
     <row r="33" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A33" s="39">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="85"/>
       <c r="C33" s="82"/>
@@ -13222,7 +13249,7 @@
     </row>
     <row r="34" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="85"/>
       <c r="C34" s="82"/>
@@ -13239,7 +13266,7 @@
     </row>
     <row r="35" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A35" s="39">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="85"/>
       <c r="C35" s="82"/>
@@ -13256,7 +13283,7 @@
     </row>
     <row r="36" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="85"/>
       <c r="C36" s="82"/>
@@ -13273,7 +13300,7 @@
     </row>
     <row r="37" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A37" s="39">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="85"/>
       <c r="C37" s="82"/>
@@ -13290,7 +13317,7 @@
     </row>
     <row r="38" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A38" s="39">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="85"/>
       <c r="C38" s="82"/>
@@ -13307,7 +13334,7 @@
     </row>
     <row r="39" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A39" s="39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="85"/>
       <c r="C39" s="82"/>
@@ -13324,7 +13351,7 @@
     </row>
     <row r="40" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A40" s="39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="85"/>
       <c r="C40" s="82"/>
@@ -13341,7 +13368,7 @@
     </row>
     <row r="41" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A41" s="39">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="85"/>
       <c r="C41" s="82"/>
@@ -13358,7 +13385,7 @@
     </row>
     <row r="42" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A42" s="39">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="85"/>
       <c r="C42" s="82"/>
@@ -13375,7 +13402,7 @@
     </row>
     <row r="43" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A43" s="39">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="85"/>
       <c r="C43" s="82"/>
@@ -13392,7 +13419,7 @@
     </row>
     <row r="44" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A44" s="39">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="85"/>
       <c r="C44" s="82"/>
@@ -13409,7 +13436,7 @@
     </row>
     <row r="45" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A45" s="39">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="85"/>
       <c r="C45" s="82"/>
@@ -13423,6 +13450,23 @@
       <c r="K45" s="84"/>
       <c r="L45" s="85"/>
       <c r="M45" s="85"/>
+    </row>
+    <row r="46" spans="1:13" ht="27" x14ac:dyDescent="0.25">
+      <c r="A46" s="39">
+        <v>43</v>
+      </c>
+      <c r="B46" s="85"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="84"/>
+      <c r="J46" s="84"/>
+      <c r="K46" s="84"/>
+      <c r="L46" s="85"/>
+      <c r="M46" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
update n.04 + n.35
</commit_message>
<xml_diff>
--- a/1404.xlsx
+++ b/1404.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chaparsar.RRS\1404\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91811B08-B4E1-495B-92D9-6E2352945A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D925E60-8167-4B97-B250-97719147CF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N.01 صفحه اصلی" sheetId="1" r:id="rId1"/>
@@ -19,27 +19,28 @@
     <sheet name="N.04 دفتر روزانه" sheetId="32" r:id="rId4"/>
     <sheet name="فرم های خام N.05" sheetId="11" r:id="rId5"/>
     <sheet name="اطلاعات حساب های ایستگاه N.06" sheetId="14" r:id="rId6"/>
-    <sheet name="مدیریت زونکن یک" sheetId="5" r:id="rId7"/>
-    <sheet name="مدیریت زونکن دو" sheetId="6" r:id="rId8"/>
-    <sheet name="N.21 حواله کود مزرعه و باغ" sheetId="25" r:id="rId9"/>
-    <sheet name="N3 زونکن سه" sheetId="8" r:id="rId10"/>
-    <sheet name="N.31 خرید کود باغ مرکبات" sheetId="31" r:id="rId11"/>
-    <sheet name="لیست مصالح دیوارکشیN.32" sheetId="24" r:id="rId12"/>
-    <sheet name="لیست کارگری دیوارکشیN.33" sheetId="23" r:id="rId13"/>
-    <sheet name="N.34 علی الحساب موقت" sheetId="13" r:id="rId14"/>
-    <sheet name="N.35 تنخواه پیمانکاری دیوارکشی" sheetId="22" r:id="rId15"/>
-    <sheet name="سایر فاکتورهای پرداخت شده" sheetId="16" r:id="rId16"/>
-    <sheet name="خلاصه وضعیت" sheetId="12" r:id="rId17"/>
-    <sheet name="دفتر تنخواه" sheetId="15" r:id="rId18"/>
-    <sheet name="زونکن سه - تنخواه - اداری" sheetId="20" r:id="rId19"/>
-    <sheet name="زونکن سه - تنخواه - قبوض" sheetId="19" r:id="rId20"/>
-    <sheet name="زونکن سه - تنخواه - فرم پذیرایی" sheetId="9" r:id="rId21"/>
-    <sheet name="زونکن سه - تنخواه - سوخت" sheetId="18" r:id="rId22"/>
-    <sheet name="زونکن سه - بایگانی - پذیرایی" sheetId="10" r:id="rId23"/>
-    <sheet name="مدیریت زونکن چهار" sheetId="7" r:id="rId24"/>
-    <sheet name="زونکن چهار - لیست مرخص روزانه" sheetId="28" r:id="rId25"/>
-    <sheet name="لیست فعالیت ماهانه همکاران شرکت" sheetId="30" r:id="rId26"/>
-    <sheet name="زونکن سه - لیست مرخص ساعتی" sheetId="29" r:id="rId27"/>
+    <sheet name="زونکن یک N1" sheetId="5" r:id="rId7"/>
+    <sheet name="ظهور خوشه N.11" sheetId="34" r:id="rId8"/>
+    <sheet name="مدیریت زونکن دو" sheetId="6" r:id="rId9"/>
+    <sheet name="N.21 حواله کود مزرعه و باغ" sheetId="25" r:id="rId10"/>
+    <sheet name="N3 زونکن سه" sheetId="8" r:id="rId11"/>
+    <sheet name="N.31 خرید کود باغ مرکبات" sheetId="31" r:id="rId12"/>
+    <sheet name="لیست مصالح دیوارکشیN.32" sheetId="24" r:id="rId13"/>
+    <sheet name="لیست کارگری دیوارکشیN.33" sheetId="23" r:id="rId14"/>
+    <sheet name="N.34 علی الحساب موقت" sheetId="13" r:id="rId15"/>
+    <sheet name="N.35 تنخواه پیمانکاری دیوارکشی" sheetId="22" r:id="rId16"/>
+    <sheet name="سایر فاکتورهای پرداخت شده" sheetId="16" r:id="rId17"/>
+    <sheet name="خلاصه وضعیت" sheetId="12" r:id="rId18"/>
+    <sheet name="دفتر تنخواه" sheetId="15" r:id="rId19"/>
+    <sheet name="زونکن سه - تنخواه - اداری" sheetId="20" r:id="rId20"/>
+    <sheet name="زونکن سه - تنخواه - قبوض" sheetId="19" r:id="rId21"/>
+    <sheet name="زونکن سه - تنخواه - فرم پذیرایی" sheetId="9" r:id="rId22"/>
+    <sheet name="زونکن سه - تنخواه - سوخت" sheetId="18" r:id="rId23"/>
+    <sheet name="زونکن سه - بایگانی - پذیرایی" sheetId="10" r:id="rId24"/>
+    <sheet name="مدیریت زونکن چهار" sheetId="7" r:id="rId25"/>
+    <sheet name="زونکن چهار - لیست مرخص روزانه" sheetId="28" r:id="rId26"/>
+    <sheet name="لیست فعالیت ماهانه همکاران شرکت" sheetId="30" r:id="rId27"/>
+    <sheet name="زونکن سه - لیست مرخص ساعتی" sheetId="29" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="307">
   <si>
     <t>اکسل مدیریتی ایستگاه تحقیقات برنج شهید شیرودی تنکابن سال 1404</t>
   </si>
@@ -938,17 +939,63 @@
   </si>
   <si>
     <t>هوشنگ کیائی + بهرام</t>
+  </si>
+  <si>
+    <t>ظهور خوشه</t>
+  </si>
+  <si>
+    <t>ارتفاع بوته تعداد پنجه</t>
+  </si>
+  <si>
+    <t>وزن درصد رطوبت</t>
+  </si>
+  <si>
+    <t>وزن هزاردانه</t>
+  </si>
+  <si>
+    <t>آمل - ناحیه ای</t>
+  </si>
+  <si>
+    <t>تاریخ نشاکاری :</t>
+  </si>
+  <si>
+    <t>نام لاین</t>
+  </si>
+  <si>
+    <t>50 درصد گلدهی</t>
+  </si>
+  <si>
+    <t>زمان رسیدن</t>
+  </si>
+  <si>
+    <t>ملاحظات</t>
+  </si>
+  <si>
+    <t>جدول ظهور خوشه</t>
+  </si>
+  <si>
+    <t>نام محقق</t>
+  </si>
+  <si>
+    <t>تعداد تیمار</t>
+  </si>
+  <si>
+    <t>تفاضل تاریخ نشاکاری و پنجاه درصد گلدهی بعلاوه 30 روز برابر با زمان رسیدن</t>
+  </si>
+  <si>
+    <t>1404/02/10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0000\/00\/00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1075,6 +1122,26 @@
     <font>
       <sz val="14"/>
       <name val="B Titr"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="B Zar"/>
       <charset val="178"/>
     </font>
   </fonts>
@@ -1212,7 +1279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1522,13 +1589,191 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1822,6 +2067,63 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1922,6 +2224,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4367,7 +4687,7 @@
   <dimension ref="D2:L8"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4381,16 +4701,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:12" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4471,6 +4791,485 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2DB39D-3131-4E2F-B906-B453417A2FF8}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:O28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="9" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="25.140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="6"/>
+    <col min="12" max="12" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="I2" s="162" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="163"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="I3" s="162" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" s="163"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="I4" s="164" t="s">
+        <v>143</v>
+      </c>
+      <c r="J4" s="165"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A7" s="122" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A9" s="39">
+        <v>1</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="21">
+        <v>450</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A10" s="39">
+        <v>2</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="21">
+        <v>100</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A11" s="39">
+        <v>3</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="21">
+        <v>100</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="39">
+        <v>4</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" s="21">
+        <v>100</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="27" x14ac:dyDescent="0.25">
+      <c r="A13" s="39">
+        <v>5</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="21">
+        <v>100</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="27" x14ac:dyDescent="0.25">
+      <c r="A14" s="39">
+        <v>6</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E14" s="39">
+        <v>600</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="27" x14ac:dyDescent="0.25">
+      <c r="A15" s="39">
+        <v>7</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E15" s="39">
+        <v>100</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="27" x14ac:dyDescent="0.25">
+      <c r="A16" s="39">
+        <v>8</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E16" s="39">
+        <v>600</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A17" s="39">
+        <v>9</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E17" s="39">
+        <v>100</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A18" s="39">
+        <v>10</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A19" s="39">
+        <v>11</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+    </row>
+    <row r="20" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A20" s="39">
+        <v>12</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A21" s="39">
+        <v>13</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+    </row>
+    <row r="22" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A22" s="39">
+        <v>14</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+    </row>
+    <row r="23" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A23" s="39">
+        <v>15</v>
+      </c>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+    </row>
+    <row r="24" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A24" s="39">
+        <v>16</v>
+      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A25" s="39">
+        <v>17</v>
+      </c>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+    </row>
+    <row r="26" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A26" s="39">
+        <v>18</v>
+      </c>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+    </row>
+    <row r="27" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A27" s="39">
+        <v>19</v>
+      </c>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+    </row>
+    <row r="28" spans="1:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="A28" s="39">
+        <v>20</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A7:E7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="L2" location="'صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{646D7D3D-BFDF-4DDD-9D6A-1A131F6BC3F2}"/>
+    <hyperlink ref="I2:J2" location="'مدیریت زونکن دو'!A1" display="زونکن شماره دو" xr:uid="{E2DA4D76-2DD8-468F-BC85-1193DCE6296C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57F183A-3386-450D-AE91-F3DA30B67E25}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -4500,11 +5299,11 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="141" t="s">
+      <c r="G2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="142"/>
-      <c r="I2" s="143"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="168"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -4512,11 +5311,11 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="141" t="s">
+      <c r="G3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="142"/>
-      <c r="I3" s="143"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="168"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -4525,12 +5324,12 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="144" t="s">
+      <c r="B5" s="169" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="145"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="146"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="171"/>
       <c r="G5" s="5" t="s">
         <v>212</v>
       </c>
@@ -4694,7 +5493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23092EF-9DF4-42EA-9EF2-6FB21114714F}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
@@ -4735,10 +5534,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="141" t="s">
+      <c r="H2" s="166" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="143"/>
+      <c r="I2" s="168"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -4754,8 +5553,8 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="143"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="168"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -4768,10 +5567,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="147" t="s">
+      <c r="H4" s="172" t="s">
         <v>215</v>
       </c>
-      <c r="I4" s="148"/>
+      <c r="I4" s="173"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -4800,12 +5599,12 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
       <c r="E7" s="73"/>
       <c r="F7" s="9"/>
       <c r="G7" s="6"/>
@@ -5154,7 +5953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F2A4A-1ADA-42DA-84DF-FB5510BE189F}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -5198,10 +5997,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="143"/>
+      <c r="J2" s="168"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -5218,10 +6017,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="141" t="s">
+      <c r="I3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="143"/>
+      <c r="J3" s="168"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -5235,10 +6034,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="147" t="s">
+      <c r="I4" s="172" t="s">
         <v>145</v>
       </c>
-      <c r="J4" s="148"/>
+      <c r="J4" s="173"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -5269,21 +6068,21 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
       <c r="F7" s="61"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="149" t="s">
+      <c r="I7" s="174" t="s">
         <v>151</v>
       </c>
-      <c r="J7" s="149"/>
-      <c r="K7" s="149"/>
+      <c r="J7" s="174"/>
+      <c r="K7" s="174"/>
       <c r="L7" s="28"/>
     </row>
     <row r="8" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -5617,15 +6416,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECC67F4-E01F-456A-965C-D1525789CDAC}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -5661,10 +6460,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="143"/>
+      <c r="J2" s="168"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -5681,10 +6480,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="141" t="s">
+      <c r="I3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="143"/>
+      <c r="J3" s="168"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -5698,10 +6497,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="147" t="s">
+      <c r="I4" s="172" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="148"/>
+      <c r="J4" s="173"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -5732,13 +6531,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
       <c r="F7" s="60"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
@@ -6036,7 +6835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A001D87-B52D-4BBB-825A-A2D9C74DF962}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -6080,10 +6879,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="143"/>
+      <c r="J2" s="168"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -6100,10 +6899,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="141" t="s">
+      <c r="I3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="143"/>
+      <c r="J3" s="168"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -6117,10 +6916,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="147" t="s">
+      <c r="I4" s="172" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="148"/>
+      <c r="J4" s="173"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -6151,13 +6950,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
       <c r="F7" s="17"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
@@ -6500,15 +7299,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7AE76D-6966-4BB9-B043-ED2E5C3B6D23}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -6548,10 +7347,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="143"/>
+      <c r="J2" s="168"/>
       <c r="K2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -6565,10 +7364,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="141" t="s">
+      <c r="I3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="143"/>
+      <c r="J3" s="168"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -6582,10 +7381,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="147" t="s">
+      <c r="I4" s="172" t="s">
         <v>129</v>
       </c>
-      <c r="J4" s="148"/>
+      <c r="J4" s="173"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -6616,13 +7415,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
       <c r="F7" s="49"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
@@ -6814,11 +7613,20 @@
       <c r="A17" s="39">
         <v>9</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
+      <c r="B17" s="85" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>265</v>
+      </c>
       <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="E17" s="39">
+        <v>907000</v>
+      </c>
+      <c r="F17" s="39">
+        <f>(F16+D17)-E17</f>
+        <v>1863000</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A18" s="39">
@@ -6947,7 +7755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03590E6F-F524-4F8C-ACD9-635A648ABCF8}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -6988,10 +7796,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="141" t="s">
+      <c r="H2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="143"/>
+      <c r="I2" s="168"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -7007,10 +7815,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="141" t="s">
+      <c r="H3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="143"/>
+      <c r="I3" s="168"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -7023,10 +7831,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="147" t="s">
+      <c r="H4" s="172" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="148"/>
+      <c r="I4" s="173"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -7041,13 +7849,13 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:14" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
       <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -7184,7 +7992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C5079D-A085-4F31-926D-1D8B6D498E67}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -7219,10 +8027,10 @@
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-      <c r="F2" s="141" t="s">
+      <c r="F2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="143"/>
+      <c r="G2" s="168"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4" t="s">
         <v>10</v>
@@ -7236,10 +8044,10 @@
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="F3" s="141" t="s">
+      <c r="F3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="143"/>
+      <c r="G3" s="168"/>
       <c r="H3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -7250,10 +8058,10 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="F4" s="147" t="s">
+      <c r="F4" s="172" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="148"/>
+      <c r="G4" s="173"/>
       <c r="H4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -7266,11 +8074,11 @@
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:12" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="123"/>
       <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:12" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -7347,10 +8155,10 @@
       <c r="C12" s="22"/>
     </row>
     <row r="13" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="150" t="s">
+      <c r="A13" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="151"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="24">
         <f>SUM(C9:C12)</f>
         <v>0</v>
@@ -7373,7 +8181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397A8150-4C95-4F03-85CC-EA5E0B56188A}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -7415,10 +8223,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="143"/>
+      <c r="J2" s="168"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -7435,10 +8243,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="141" t="s">
+      <c r="I3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="143"/>
+      <c r="J3" s="168"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -7452,10 +8260,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="147" t="s">
+      <c r="I4" s="172" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="148"/>
+      <c r="J4" s="173"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -7486,13 +8294,13 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
       <c r="F7" s="27"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
@@ -7774,7 +8582,176 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C1A410-FC7C-489E-923F-4169D4A63975}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="121" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+    </row>
+    <row r="4" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="96" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K5" s="97" t="s">
+        <v>232</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K6" s="98" t="s">
+        <v>276</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="K7" s="81" t="s">
+        <v>241</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:I3"/>
+  </mergeCells>
+  <phoneticPr fontId="17" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H4" location="'مدیریت زونکن یک'!A1" display="یک" xr:uid="{5FE9FE58-3527-4026-9FE9-21315B02564B}"/>
+    <hyperlink ref="F4" location="'مدیریت زونکن دو'!A1" display="دو" xr:uid="{2E55D6D8-D527-4D04-8025-712BFAD0DAFB}"/>
+    <hyperlink ref="D4" location="'زونکن سه - تنخواه'!A1" display="سه" xr:uid="{863EFE16-BC07-43F9-8CB6-B9C4C8FE3F71}"/>
+    <hyperlink ref="B4" location="'مدیریت زونکن چهار'!A1" display="چهار" xr:uid="{A032C9B8-DB95-4F3A-899B-8CE6AC6B074C}"/>
+    <hyperlink ref="K8" location="'فرم های خام'!A1" display="فرم های خام" xr:uid="{B61CBFE3-0502-4A24-87C1-B75EE7D3D861}"/>
+    <hyperlink ref="K9" location="'اطلاعات حساب های ایستگاه'!A1" display="اطلاعات حساب های ایستگاه" xr:uid="{62E8C4C2-FBC7-4756-BE75-9B163AA32561}"/>
+    <hyperlink ref="E4" location="'زونکن سه - تنخواه'!A1" display="تنخواه" xr:uid="{55E349AD-7083-44E2-B6AB-FAEB496FFA58}"/>
+    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{8DB2D9B0-82A4-4AA0-8093-2DB0A2D6849B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AF6ECC-C25D-4AE4-9D51-65D2BBBC0054}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -7828,10 +8805,10 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
-      <c r="L2" s="141" t="s">
+      <c r="L2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="143"/>
+      <c r="M2" s="168"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4" t="s">
         <v>10</v>
@@ -7851,10 +8828,10 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
-      <c r="L3" s="141" t="s">
+      <c r="L3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="143"/>
+      <c r="M3" s="168"/>
       <c r="N3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -7871,10 +8848,10 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="L4" s="147" t="s">
+      <c r="L4" s="172" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="148"/>
+      <c r="M4" s="173"/>
       <c r="N4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -7891,10 +8868,10 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="L5" s="152" t="s">
+      <c r="L5" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="153"/>
+      <c r="M5" s="178"/>
       <c r="N5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -7913,16 +8890,16 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:18" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
       <c r="I7" s="74" t="s">
         <v>207</v>
       </c>
@@ -8297,176 +9274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C1A410-FC7C-489E-923F-4169D4A63975}">
-  <sheetPr>
-    <tabColor theme="4" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:O9"/>
-  <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="G2" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="102" t="s">
-        <v>233</v>
-      </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-    </row>
-    <row r="4" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="96" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K5" s="97" t="s">
-        <v>232</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="K6" s="98" t="s">
-        <v>276</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="K7" s="81" t="s">
-        <v>241</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:I3"/>
-  </mergeCells>
-  <phoneticPr fontId="17" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="H4" location="'مدیریت زونکن یک'!A1" display="یک" xr:uid="{5FE9FE58-3527-4026-9FE9-21315B02564B}"/>
-    <hyperlink ref="F4" location="'مدیریت زونکن دو'!A1" display="دو" xr:uid="{2E55D6D8-D527-4D04-8025-712BFAD0DAFB}"/>
-    <hyperlink ref="D4" location="'زونکن سه - تنخواه'!A1" display="سه" xr:uid="{863EFE16-BC07-43F9-8CB6-B9C4C8FE3F71}"/>
-    <hyperlink ref="B4" location="'مدیریت زونکن چهار'!A1" display="چهار" xr:uid="{A032C9B8-DB95-4F3A-899B-8CE6AC6B074C}"/>
-    <hyperlink ref="K8" location="'فرم های خام'!A1" display="فرم های خام" xr:uid="{B61CBFE3-0502-4A24-87C1-B75EE7D3D861}"/>
-    <hyperlink ref="K9" location="'اطلاعات حساب های ایستگاه'!A1" display="اطلاعات حساب های ایستگاه" xr:uid="{62E8C4C2-FBC7-4756-BE75-9B163AA32561}"/>
-    <hyperlink ref="E4" location="'زونکن سه - تنخواه'!A1" display="تنخواه" xr:uid="{55E349AD-7083-44E2-B6AB-FAEB496FFA58}"/>
-    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{8DB2D9B0-82A4-4AA0-8093-2DB0A2D6849B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611E4142-FA06-4F8C-8479-92BC84077D6A}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -8513,10 +9321,10 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="K2" s="141" t="s">
+      <c r="K2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="143"/>
+      <c r="L2" s="168"/>
       <c r="M2" s="3"/>
       <c r="N2" s="4" t="s">
         <v>10</v>
@@ -8535,10 +9343,10 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="K3" s="141" t="s">
+      <c r="K3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="143"/>
+      <c r="L3" s="168"/>
       <c r="M3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
@@ -8554,10 +9362,10 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="K4" s="147" t="s">
+      <c r="K4" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="148"/>
+      <c r="L4" s="173"/>
       <c r="M4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -8573,10 +9381,10 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="K5" s="152" t="s">
+      <c r="K5" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="153"/>
+      <c r="L5" s="178"/>
       <c r="M5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -8594,16 +9402,16 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:17" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:17" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -8943,7 +9751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74664C7B-AF9D-4AAA-84CE-5A79A28E0748}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -8984,10 +9792,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="141" t="s">
+      <c r="H2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="143"/>
+      <c r="I2" s="168"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -9003,10 +9811,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="141" t="s">
+      <c r="H3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="143"/>
+      <c r="I3" s="168"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -9019,10 +9827,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="147" t="s">
+      <c r="H4" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="148"/>
+      <c r="I4" s="173"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -9035,10 +9843,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="152" t="s">
+      <c r="H5" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="153"/>
+      <c r="I5" s="178"/>
       <c r="J5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -9053,13 +9861,13 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -9303,13 +10111,13 @@
       <c r="E29" s="16"/>
     </row>
     <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A41" s="103" t="s">
+      <c r="A41" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="103"/>
-      <c r="C41" s="103"/>
-      <c r="D41" s="103"/>
-      <c r="E41" s="103"/>
+      <c r="B41" s="122"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="122"/>
+      <c r="E41" s="122"/>
     </row>
     <row r="42" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
@@ -9540,7 +10348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E05E92-F6C6-4B7D-8902-B6A7A2B70891}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -9589,10 +10397,10 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="J2" s="141" t="s">
+      <c r="J2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="143"/>
+      <c r="K2" s="168"/>
       <c r="L2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -9607,10 +10415,10 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="J3" s="141" t="s">
+      <c r="J3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="143"/>
+      <c r="K3" s="168"/>
       <c r="L3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -9625,10 +10433,10 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="J4" s="147" t="s">
+      <c r="J4" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="148"/>
+      <c r="K4" s="173"/>
       <c r="L4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -9643,10 +10451,10 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="J5" s="152" t="s">
+      <c r="J5" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="153"/>
+      <c r="K5" s="178"/>
       <c r="L5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -9663,15 +10471,15 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:16" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="122" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -9975,7 +10783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4824894-99A7-468B-A8A6-2B99A48AF766}">
   <sheetPr>
     <tabColor theme="8" tint="0.59999389629810485"/>
@@ -10018,10 +10826,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="141" t="s">
+      <c r="H2" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="143"/>
+      <c r="I2" s="168"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -10034,10 +10842,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="141" t="s">
+      <c r="H3" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="143"/>
+      <c r="I3" s="168"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -10050,10 +10858,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="152" t="s">
+      <c r="H4" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="153"/>
+      <c r="I4" s="178"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -10066,10 +10874,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="147" t="s">
+      <c r="H5" s="172" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="148"/>
+      <c r="I5" s="173"/>
       <c r="J5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -10093,13 +10901,13 @@
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -10410,7 +11218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F6B1EE-0CDB-40D5-AA97-407B3D9B5EAB}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -10436,10 +11244,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="154" t="s">
+      <c r="K2" s="179" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="155"/>
+      <c r="L2" s="180"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -10486,7 +11294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306C899E-EDF2-4E78-9E17-5B8A229DB2C4}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
@@ -10529,10 +11337,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="129" t="s">
+      <c r="H2" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="130"/>
+      <c r="I2" s="149"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -10545,10 +11353,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="154" t="s">
+      <c r="H3" s="179" t="s">
         <v>165</v>
       </c>
-      <c r="I3" s="155"/>
+      <c r="I3" s="180"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -10563,13 +11371,13 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="122" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:14" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -10885,7 +11693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930F3AE4-F05A-41F7-94FE-13D5DDEE4B2A}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
@@ -10927,10 +11735,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="129" t="s">
+      <c r="H2" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="130"/>
+      <c r="I2" s="149"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -10942,10 +11750,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="154" t="s">
+      <c r="H3" s="179" t="s">
         <v>175</v>
       </c>
-      <c r="I3" s="155"/>
+      <c r="I3" s="180"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -10959,20 +11767,20 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="27" x14ac:dyDescent="0.25">
-      <c r="B5" s="157" t="s">
+      <c r="B5" s="182" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
+      <c r="C5" s="182"/>
+      <c r="D5" s="182"/>
+      <c r="E5" s="182"/>
     </row>
     <row r="6" spans="1:14" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="158" t="s">
+      <c r="A6" s="183" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="158"/>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="183"/>
+      <c r="C6" s="183"/>
+      <c r="D6" s="183"/>
       <c r="E6" s="72"/>
       <c r="F6" s="72"/>
       <c r="G6" s="72"/>
@@ -11018,11 +11826,11 @@
       <c r="J9"/>
     </row>
     <row r="10" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="156" t="s">
+      <c r="B10" s="181" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="156"/>
-      <c r="D10" s="156"/>
+      <c r="C10" s="181"/>
+      <c r="D10" s="181"/>
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="71"/>
@@ -11171,11 +11979,11 @@
       <c r="J20" s="72"/>
     </row>
     <row r="21" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="156" t="s">
+      <c r="B21" s="181" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="156"/>
-      <c r="D21" s="156"/>
+      <c r="C21" s="181"/>
+      <c r="D21" s="181"/>
       <c r="E21" s="72"/>
       <c r="F21" s="72"/>
       <c r="G21" s="72"/>
@@ -11217,20 +12025,20 @@
       <c r="J24" s="68"/>
     </row>
     <row r="25" spans="1:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="B25" s="157" t="s">
+      <c r="B25" s="182" t="s">
         <v>199</v>
       </c>
-      <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="157"/>
+      <c r="C25" s="182"/>
+      <c r="D25" s="182"/>
+      <c r="E25" s="182"/>
     </row>
     <row r="26" spans="1:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="A26" s="158" t="s">
+      <c r="A26" s="183" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="158"/>
-      <c r="C26" s="158"/>
-      <c r="D26" s="158"/>
+      <c r="B26" s="183"/>
+      <c r="C26" s="183"/>
+      <c r="D26" s="183"/>
     </row>
     <row r="27" spans="1:10" ht="27" x14ac:dyDescent="0.25">
       <c r="B27"/>
@@ -11254,11 +12062,11 @@
       <c r="D29"/>
     </row>
     <row r="30" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="156" t="s">
+      <c r="B30" s="181" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="156"/>
-      <c r="D30" s="156"/>
+      <c r="C30" s="181"/>
+      <c r="D30" s="181"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:10" ht="27" x14ac:dyDescent="0.55000000000000004">
@@ -11352,11 +12160,11 @@
       <c r="D40" s="72"/>
     </row>
     <row r="41" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="156" t="s">
+      <c r="B41" s="181" t="s">
         <v>188</v>
       </c>
-      <c r="C41" s="156"/>
-      <c r="D41" s="156"/>
+      <c r="C41" s="181"/>
+      <c r="D41" s="181"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -11381,7 +12189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043F82A5-E35F-4FD7-BC9C-13B5DFE62BF2}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
@@ -11419,10 +12227,10 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="G2" s="129" t="s">
+      <c r="G2" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="130"/>
+      <c r="H2" s="149"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4" t="s">
         <v>10</v>
@@ -11437,10 +12245,10 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="G3" s="154" t="s">
+      <c r="G3" s="179" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="155"/>
+      <c r="H3" s="180"/>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -11454,12 +12262,12 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="122" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -11777,12 +12585,12 @@
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
     </row>
     <row r="4" spans="1:6" s="7" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -11828,13 +12636,13 @@
     </row>
     <row r="7" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="122" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
       <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12209,8 +13017,8 @@
       <c r="A122" s="20"/>
     </row>
     <row r="125" spans="1:2" ht="27" x14ac:dyDescent="0.25">
-      <c r="A125" s="103"/>
-      <c r="B125" s="103"/>
+      <c r="A125" s="122"/>
+      <c r="B125" s="122"/>
     </row>
     <row r="126" spans="1:2" ht="27" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
@@ -12322,8 +13130,8 @@
   <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12344,47 +13152,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="107" t="s">
+      <c r="B1" s="128"/>
+      <c r="C1" s="126" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
     </row>
     <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="140" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="129" t="s">
         <v>267</v>
       </c>
-      <c r="D2" s="111"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="113" t="s">
+      <c r="D2" s="130"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="132" t="s">
         <v>268</v>
       </c>
-      <c r="G2" s="114"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="116" t="s">
+      <c r="G2" s="133"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="135" t="s">
         <v>269</v>
       </c>
-      <c r="J2" s="117"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="105" t="s">
+      <c r="J2" s="136"/>
+      <c r="K2" s="137"/>
+      <c r="L2" s="124" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="90" t="s">
@@ -12392,8 +13200,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="122"/>
-      <c r="B3" s="120"/>
+      <c r="A3" s="141"/>
+      <c r="B3" s="139"/>
       <c r="C3" s="91" t="s">
         <v>270</v>
       </c>
@@ -12421,7 +13229,7 @@
       <c r="K3" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="106"/>
+      <c r="L3" s="125"/>
       <c r="M3" s="90" t="s">
         <v>274</v>
       </c>
@@ -12496,7 +13304,7 @@
       <c r="F6" s="83"/>
       <c r="G6" s="83"/>
       <c r="H6" s="83">
-        <f t="shared" ref="H6:H27" si="0">(H5+F6)-G6</f>
+        <f t="shared" ref="H6:H30" si="0">(H5+F6)-G6</f>
         <v>0</v>
       </c>
       <c r="I6" s="84"/>
@@ -13149,7 +13957,10 @@
       <c r="E28" s="82"/>
       <c r="F28" s="83"/>
       <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
+      <c r="H28" s="83">
+        <f t="shared" si="0"/>
+        <v>2770000</v>
+      </c>
       <c r="I28" s="84"/>
       <c r="J28" s="84">
         <v>8000000</v>
@@ -13177,7 +13988,10 @@
       <c r="E29" s="82"/>
       <c r="F29" s="83"/>
       <c r="G29" s="83"/>
-      <c r="H29" s="83"/>
+      <c r="H29" s="83">
+        <f t="shared" si="0"/>
+        <v>2770000</v>
+      </c>
       <c r="I29" s="84"/>
       <c r="J29" s="84">
         <v>5267000</v>
@@ -13197,18 +14011,29 @@
       <c r="A30" s="39">
         <v>27</v>
       </c>
-      <c r="B30" s="85"/>
+      <c r="B30" s="85" t="s">
+        <v>306</v>
+      </c>
       <c r="C30" s="82"/>
       <c r="D30" s="82"/>
       <c r="E30" s="82"/>
       <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
+      <c r="G30" s="83">
+        <v>907000</v>
+      </c>
+      <c r="H30" s="83">
+        <f t="shared" si="0"/>
+        <v>1863000</v>
+      </c>
       <c r="I30" s="84"/>
       <c r="J30" s="84"/>
       <c r="K30" s="84"/>
-      <c r="L30" s="85"/>
-      <c r="M30" s="85"/>
+      <c r="L30" s="85" t="s">
+        <v>266</v>
+      </c>
+      <c r="M30" s="85" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="31" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
@@ -13529,10 +14354,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="124"/>
+      <c r="B1" s="143"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -13545,10 +14370,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="125" t="s">
+      <c r="H2" s="144" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="126"/>
+      <c r="I2" s="145"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -13561,10 +14386,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="127" t="s">
+      <c r="H3" s="146" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="128"/>
+      <c r="I3" s="147"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -13593,13 +14418,13 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:13" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -13868,13 +14693,13 @@
       <c r="M30" s="6"/>
     </row>
     <row r="33" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A33" s="103" t="s">
+      <c r="A33" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="103"/>
-      <c r="C33" s="103"/>
-      <c r="D33" s="103"/>
-      <c r="E33" s="103"/>
+      <c r="B33" s="122"/>
+      <c r="C33" s="122"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="122"/>
       <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" ht="27" x14ac:dyDescent="0.25">
@@ -14098,14 +14923,14 @@
       <c r="F54" s="21"/>
     </row>
     <row r="57" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A57" s="104" t="s">
+      <c r="A57" s="123" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="104"/>
-      <c r="C57" s="104"/>
-      <c r="D57" s="104"/>
-      <c r="E57" s="104"/>
-      <c r="F57" s="104"/>
+      <c r="B57" s="123"/>
+      <c r="C57" s="123"/>
+      <c r="D57" s="123"/>
+      <c r="E57" s="123"/>
+      <c r="F57" s="123"/>
     </row>
     <row r="58" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
@@ -14327,12 +15152,12 @@
       <c r="F78" s="20"/>
     </row>
     <row r="82" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A82" s="104" t="s">
+      <c r="A82" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="B82" s="104"/>
-      <c r="C82" s="104"/>
-      <c r="D82" s="104"/>
+      <c r="B82" s="123"/>
+      <c r="C82" s="123"/>
+      <c r="D82" s="123"/>
     </row>
     <row r="83" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
@@ -14509,15 +15334,15 @@
       <c r="D103" s="22"/>
     </row>
     <row r="106" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A106" s="103" t="s">
+      <c r="A106" s="122" t="s">
         <v>101</v>
       </c>
-      <c r="B106" s="103"/>
-      <c r="C106" s="103"/>
-      <c r="D106" s="103"/>
-      <c r="E106" s="103"/>
-      <c r="F106" s="103"/>
-      <c r="G106" s="103"/>
+      <c r="B106" s="122"/>
+      <c r="C106" s="122"/>
+      <c r="D106" s="122"/>
+      <c r="E106" s="122"/>
+      <c r="F106" s="122"/>
+      <c r="G106" s="122"/>
     </row>
     <row r="107" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
@@ -14767,16 +15592,16 @@
       <c r="G127" s="20"/>
     </row>
     <row r="130" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A130" s="103" t="s">
+      <c r="A130" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="B130" s="103"/>
-      <c r="C130" s="103"/>
-      <c r="D130" s="103"/>
-      <c r="E130" s="103"/>
-      <c r="F130" s="103"/>
-      <c r="G130" s="103"/>
-      <c r="H130" s="103"/>
+      <c r="B130" s="122"/>
+      <c r="C130" s="122"/>
+      <c r="D130" s="122"/>
+      <c r="E130" s="122"/>
+      <c r="F130" s="122"/>
+      <c r="G130" s="122"/>
+      <c r="H130" s="122"/>
     </row>
     <row r="131" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
@@ -15045,13 +15870,13 @@
       <c r="H151" s="10"/>
     </row>
     <row r="155" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A155" s="103" t="s">
+      <c r="A155" s="122" t="s">
         <v>143</v>
       </c>
-      <c r="B155" s="103"/>
-      <c r="C155" s="103"/>
-      <c r="D155" s="103"/>
-      <c r="E155" s="103"/>
+      <c r="B155" s="122"/>
+      <c r="C155" s="122"/>
+      <c r="D155" s="122"/>
+      <c r="E155" s="122"/>
       <c r="F155" s="63"/>
     </row>
     <row r="156" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -15275,13 +16100,13 @@
       <c r="F176" s="39"/>
     </row>
     <row r="179" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A179" s="103" t="s">
+      <c r="A179" s="122" t="s">
         <v>145</v>
       </c>
-      <c r="B179" s="103"/>
-      <c r="C179" s="103"/>
-      <c r="D179" s="103"/>
-      <c r="E179" s="103"/>
+      <c r="B179" s="122"/>
+      <c r="C179" s="122"/>
+      <c r="D179" s="122"/>
+      <c r="E179" s="122"/>
       <c r="F179" s="66"/>
     </row>
     <row r="180" spans="1:6" ht="27" x14ac:dyDescent="0.25">
@@ -15501,14 +16326,14 @@
       <c r="F200" s="39"/>
     </row>
     <row r="204" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A204" s="104" t="s">
+      <c r="A204" s="123" t="s">
         <v>219</v>
       </c>
-      <c r="B204" s="104"/>
-      <c r="C204" s="104"/>
-      <c r="D204" s="104"/>
-      <c r="E204" s="104"/>
-      <c r="F204" s="104"/>
+      <c r="B204" s="123"/>
+      <c r="C204" s="123"/>
+      <c r="D204" s="123"/>
+      <c r="E204" s="123"/>
+      <c r="F204" s="123"/>
     </row>
     <row r="205" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A205" s="78" t="s">
@@ -16074,16 +16899,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="124"/>
+      <c r="B1" s="143"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="129" t="s">
+      <c r="J2" s="148" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="130"/>
+      <c r="K2" s="149"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -16123,10 +16948,10 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="129" t="s">
+      <c r="J12" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="130"/>
+      <c r="K12" s="149"/>
     </row>
     <row r="13" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="2">
@@ -16197,7 +17022,7 @@
       </c>
     </row>
     <row r="24" spans="9:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="131" t="s">
+      <c r="I24" s="150" t="s">
         <v>76</v>
       </c>
       <c r="J24" s="2">
@@ -16208,7 +17033,7 @@
       </c>
     </row>
     <row r="25" spans="9:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I25" s="132"/>
+      <c r="I25" s="151"/>
       <c r="J25" s="2" t="s">
         <v>74</v>
       </c>
@@ -16239,13 +17064,16 @@
   </sheetPr>
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="9.140625" style="1"/>
-    <col min="11" max="12" width="25.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="1"/>
     <col min="14" max="14" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
@@ -16257,10 +17085,10 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="133" t="s">
+      <c r="K2" s="152" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="134"/>
+      <c r="L2" s="153"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -16269,34 +17097,32 @@
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="K4" s="101" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K5" s="2" t="s">
-        <v>1</v>
+        <v>294</v>
       </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K6" s="2" t="s">
-        <v>2</v>
+        <v>293</v>
       </c>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K7" s="2" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="2" t="s">
-        <v>4</v>
+        <v>295</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -16312,6 +17138,291 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F697B8F-1EC9-4454-8B53-8BF8C96D3EB4}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:N24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="25.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="6"/>
+    <col min="11" max="11" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="H2" s="154" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="155"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="H3" s="156" t="s">
+        <v>292</v>
+      </c>
+      <c r="I3" s="157"/>
+      <c r="J3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="158" t="s">
+        <v>302</v>
+      </c>
+      <c r="B6" s="158"/>
+      <c r="C6" s="158"/>
+      <c r="D6" s="158"/>
+      <c r="E6" s="158"/>
+    </row>
+    <row r="7" spans="1:14" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="102" t="s">
+        <v>303</v>
+      </c>
+      <c r="B7" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="C7" s="104" t="s">
+        <v>304</v>
+      </c>
+      <c r="D7" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="E7" s="106">
+        <v>14030302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="108" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" s="109" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="109" t="s">
+        <v>299</v>
+      </c>
+      <c r="D9" s="109" t="s">
+        <v>300</v>
+      </c>
+      <c r="E9" s="110" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="111">
+        <v>1</v>
+      </c>
+      <c r="B10" s="112">
+        <v>14030428</v>
+      </c>
+      <c r="C10" s="112">
+        <v>14030503</v>
+      </c>
+      <c r="D10" s="113" t="e">
+        <f ca="1">(Diff($E$7,C10))+30</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E10" s="114"/>
+      <c r="G10" s="159" t="s">
+        <v>305</v>
+      </c>
+      <c r="H10" s="159"/>
+      <c r="I10" s="159"/>
+    </row>
+    <row r="11" spans="1:14" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="111">
+        <v>2</v>
+      </c>
+      <c r="B11" s="112">
+        <v>14030429</v>
+      </c>
+      <c r="C11" s="112">
+        <v>14030431</v>
+      </c>
+      <c r="D11" s="113" t="e">
+        <f ca="1">(Diff($E$2,C11))+30</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E11" s="114"/>
+    </row>
+    <row r="12" spans="1:14" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="111"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="114"/>
+    </row>
+    <row r="13" spans="1:14" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="111"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="114"/>
+    </row>
+    <row r="14" spans="1:14" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="111"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="114"/>
+    </row>
+    <row r="15" spans="1:14" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="111"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="114"/>
+    </row>
+    <row r="16" spans="1:14" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="114"/>
+    </row>
+    <row r="17" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="111"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="114"/>
+    </row>
+    <row r="18" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="111"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="114"/>
+    </row>
+    <row r="19" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="111"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="113"/>
+      <c r="E19" s="114"/>
+    </row>
+    <row r="20" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="111"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="114"/>
+    </row>
+    <row r="21" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="111"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="114"/>
+    </row>
+    <row r="22" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="111"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="114"/>
+    </row>
+    <row r="23" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="115"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="114"/>
+    </row>
+    <row r="24" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="116"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="119"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="G10:I10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K2" location="'صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{5F86CD0C-3EB4-448B-91D8-84638F732456}"/>
+    <hyperlink ref="H2:I2" location="'زونکن یک N1'!A1" display="زونکن شماره دو" xr:uid="{F9257ED5-3024-4D58-9025-13C2EE112160}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2048FEE-3399-40DE-A28A-5C279080E45C}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
@@ -16338,10 +17449,10 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="135" t="s">
+      <c r="K2" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="136"/>
+      <c r="L2" s="161"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -16392,483 +17503,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2DB39D-3131-4E2F-B906-B453417A2FF8}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:O28"/>
-  <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="27" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="9" customWidth="1"/>
-    <col min="7" max="7" width="32.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="25.140625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="6"/>
-    <col min="12" max="12" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="I2" s="137" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="138"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="I3" s="137" t="s">
-        <v>157</v>
-      </c>
-      <c r="J3" s="138"/>
-      <c r="K3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="I4" s="139" t="s">
-        <v>143</v>
-      </c>
-      <c r="J4" s="140"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
-        <v>1</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="E9" s="21">
-        <v>450</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
-        <v>2</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="21">
-        <v>100</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
-        <v>3</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E11" s="21">
-        <v>100</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:15" ht="27" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
-        <v>4</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="E12" s="21">
-        <v>100</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="27" x14ac:dyDescent="0.25">
-      <c r="A13" s="39">
-        <v>5</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="E13" s="21">
-        <v>100</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="27" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
-        <v>6</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>255</v>
-      </c>
-      <c r="E14" s="39">
-        <v>600</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="27" x14ac:dyDescent="0.25">
-      <c r="A15" s="39">
-        <v>7</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>255</v>
-      </c>
-      <c r="E15" s="39">
-        <v>100</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="27" x14ac:dyDescent="0.25">
-      <c r="A16" s="39">
-        <v>8</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>255</v>
-      </c>
-      <c r="E16" s="39">
-        <v>600</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A17" s="39">
-        <v>9</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>255</v>
-      </c>
-      <c r="E17" s="39">
-        <v>100</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
-        <v>10</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-    </row>
-    <row r="19" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A19" s="39">
-        <v>11</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-    </row>
-    <row r="20" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A20" s="39">
-        <v>12</v>
-      </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-    </row>
-    <row r="21" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
-        <v>13</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-    </row>
-    <row r="22" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
-        <v>14</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-    </row>
-    <row r="23" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
-        <v>15</v>
-      </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-    </row>
-    <row r="24" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A24" s="39">
-        <v>16</v>
-      </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-    </row>
-    <row r="25" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A25" s="39">
-        <v>17</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-    </row>
-    <row r="26" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A26" s="39">
-        <v>18</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-    </row>
-    <row r="27" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A27" s="39">
-        <v>19</v>
-      </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-    </row>
-    <row r="28" spans="1:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="A28" s="39">
-        <v>20</v>
-      </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A7:E7"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="L2" location="'صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{646D7D3D-BFDF-4DDD-9D6A-1A131F6BC3F2}"/>
-    <hyperlink ref="I2:J2" location="'مدیریت زونکن دو'!A1" display="زونکن شماره دو" xr:uid="{E2DA4D76-2DD8-468F-BC85-1193DCE6296C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update n.34 + n.04
</commit_message>
<xml_diff>
--- a/1404.xlsx
+++ b/1404.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chaparsar.RRS\1404\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DA3809-8A9D-4246-A6A9-92770CA631AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B712623F-15D3-4000-8CA1-222D5B1272F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N.01 صفحه اصلی" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="312">
   <si>
     <t>اکسل مدیریتی ایستگاه تحقیقات برنج شهید شیرودی تنکابن سال 1404</t>
   </si>
@@ -990,6 +990,15 @@
   </si>
   <si>
     <t>1404/02/13</t>
+  </si>
+  <si>
+    <t>1404/02/14</t>
+  </si>
+  <si>
+    <t>خرید کود اوره</t>
+  </si>
+  <si>
+    <t>قبض برق</t>
   </si>
 </sst>
 </file>
@@ -2175,15 +2184,6 @@
     <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2321,6 +2321,15 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4839,10 +4848,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="162" t="s">
+      <c r="I2" s="159" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="163"/>
+      <c r="J2" s="160"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -4859,10 +4868,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="162" t="s">
+      <c r="I3" s="159" t="s">
         <v>157</v>
       </c>
-      <c r="J3" s="163"/>
+      <c r="J3" s="160"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -4876,10 +4885,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="164" t="s">
+      <c r="I4" s="161" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="165"/>
+      <c r="J4" s="162"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -5305,11 +5314,11 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="166" t="s">
+      <c r="G2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="167"/>
-      <c r="I2" s="168"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="165"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -5317,11 +5326,11 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="166" t="s">
+      <c r="G3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="167"/>
-      <c r="I3" s="168"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="165"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -5330,12 +5339,12 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="166" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="171"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="168"/>
       <c r="G5" s="5" t="s">
         <v>212</v>
       </c>
@@ -5540,10 +5549,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="166" t="s">
+      <c r="H2" s="163" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="168"/>
+      <c r="I2" s="165"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -5559,8 +5568,8 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="168"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="165"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -5573,10 +5582,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="172" t="s">
+      <c r="H4" s="169" t="s">
         <v>215</v>
       </c>
-      <c r="I4" s="173"/>
+      <c r="I4" s="170"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -6003,10 +6012,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="166" t="s">
+      <c r="I2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="168"/>
+      <c r="J2" s="165"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -6023,10 +6032,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="166" t="s">
+      <c r="I3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="168"/>
+      <c r="J3" s="165"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -6040,10 +6049,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="172" t="s">
+      <c r="I4" s="169" t="s">
         <v>145</v>
       </c>
-      <c r="J4" s="173"/>
+      <c r="J4" s="170"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -6084,11 +6093,11 @@
       <c r="F7" s="61"/>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="174" t="s">
+      <c r="I7" s="171" t="s">
         <v>151</v>
       </c>
-      <c r="J7" s="174"/>
-      <c r="K7" s="174"/>
+      <c r="J7" s="171"/>
+      <c r="K7" s="171"/>
       <c r="L7" s="28"/>
     </row>
     <row r="8" spans="1:15" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -6441,8 +6450,8 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:E18"/>
+    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -6478,10 +6487,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="166" t="s">
+      <c r="I2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="168"/>
+      <c r="J2" s="165"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -6498,10 +6507,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="166" t="s">
+      <c r="I3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="168"/>
+      <c r="J3" s="165"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -6515,10 +6524,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="172" t="s">
+      <c r="I4" s="169" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="173"/>
+      <c r="J4" s="170"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -6893,8 +6902,8 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -6930,10 +6939,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="166" t="s">
+      <c r="I2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="168"/>
+      <c r="J2" s="165"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -6950,10 +6959,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="166" t="s">
+      <c r="I3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="168"/>
+      <c r="J3" s="165"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -6967,10 +6976,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="172" t="s">
+      <c r="I4" s="169" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="173"/>
+      <c r="J4" s="170"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -7094,7 +7103,7 @@
         <v>352000</v>
       </c>
       <c r="F11" s="39">
-        <f t="shared" ref="F11:F18" si="0">F10-E11</f>
+        <f t="shared" ref="F11:F21" si="0">F10-E11</f>
         <v>7749000</v>
       </c>
       <c r="G11" s="9"/>
@@ -7237,31 +7246,58 @@
       <c r="A19" s="39">
         <v>11</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
+      <c r="B19" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>310</v>
+      </c>
       <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="E19" s="39">
+        <v>8000000</v>
+      </c>
+      <c r="F19" s="39">
+        <f t="shared" si="0"/>
+        <v>-13832000</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
         <v>12</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
+      <c r="B20" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>311</v>
+      </c>
       <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
+      <c r="E20" s="39">
+        <v>4899000</v>
+      </c>
+      <c r="F20" s="39">
+        <f t="shared" si="0"/>
+        <v>-18731000</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
         <v>13</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
+      <c r="B21" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>121</v>
+      </c>
       <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
+      <c r="E21" s="39">
+        <v>3000000</v>
+      </c>
+      <c r="F21" s="39">
+        <f t="shared" si="0"/>
+        <v>-21731000</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
@@ -7398,10 +7434,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="166" t="s">
+      <c r="I2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="168"/>
+      <c r="J2" s="165"/>
       <c r="K2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -7415,10 +7451,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="166" t="s">
+      <c r="I3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="168"/>
+      <c r="J3" s="165"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -7432,10 +7468,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="172" t="s">
+      <c r="I4" s="169" t="s">
         <v>129</v>
       </c>
-      <c r="J4" s="173"/>
+      <c r="J4" s="170"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -7832,7 +7868,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -7865,10 +7901,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="166" t="s">
+      <c r="H2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="168"/>
+      <c r="I2" s="165"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -7884,10 +7920,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="166" t="s">
+      <c r="H3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="168"/>
+      <c r="I3" s="165"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -7900,10 +7936,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="172" t="s">
+      <c r="H4" s="169" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="173"/>
+      <c r="I4" s="170"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -8096,10 +8132,10 @@
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-      <c r="F2" s="166" t="s">
+      <c r="F2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="168"/>
+      <c r="G2" s="165"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4" t="s">
         <v>10</v>
@@ -8113,10 +8149,10 @@
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="F3" s="166" t="s">
+      <c r="F3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="168"/>
+      <c r="G3" s="165"/>
       <c r="H3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -8127,10 +8163,10 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="F4" s="172" t="s">
+      <c r="F4" s="169" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="173"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -8224,10 +8260,10 @@
       <c r="C12" s="22"/>
     </row>
     <row r="13" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="175" t="s">
+      <c r="A13" s="172" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="176"/>
+      <c r="B13" s="173"/>
       <c r="C13" s="24">
         <f>SUM(C9:C12)</f>
         <v>0</v>
@@ -8292,10 +8328,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="166" t="s">
+      <c r="I2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="168"/>
+      <c r="J2" s="165"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4" t="s">
         <v>10</v>
@@ -8312,10 +8348,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="166" t="s">
+      <c r="I3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="168"/>
+      <c r="J3" s="165"/>
       <c r="K3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -8329,10 +8365,10 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="172" t="s">
+      <c r="I4" s="169" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="173"/>
+      <c r="J4" s="170"/>
       <c r="K4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -8829,7 +8865,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B9" sqref="B9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -8874,10 +8910,10 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
-      <c r="L2" s="166" t="s">
+      <c r="L2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="168"/>
+      <c r="M2" s="165"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4" t="s">
         <v>10</v>
@@ -8897,10 +8933,10 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
-      <c r="L3" s="166" t="s">
+      <c r="L3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="168"/>
+      <c r="M3" s="165"/>
       <c r="N3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -8917,10 +8953,10 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="L4" s="172" t="s">
+      <c r="L4" s="169" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="173"/>
+      <c r="M4" s="170"/>
       <c r="N4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -8937,10 +8973,10 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="L5" s="177" t="s">
+      <c r="L5" s="174" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="178"/>
+      <c r="M5" s="175"/>
       <c r="N5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -9018,19 +9054,6 @@
       <c r="A9" s="39">
         <v>1</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39">
-        <v>3000000</v>
-      </c>
       <c r="I9" s="67" t="s">
         <v>206</v>
       </c>
@@ -9303,24 +9326,24 @@
         <v>28</v>
       </c>
       <c r="D29" s="40">
-        <f>SUM(D9:D28)</f>
+        <f>SUM(D10:D28)</f>
         <v>0</v>
       </c>
       <c r="E29" s="44">
-        <f>SUM(E9:E28)</f>
+        <f>SUM(E10:E28)</f>
         <v>0</v>
       </c>
       <c r="F29" s="44">
-        <f>SUM(F9:F28)</f>
+        <f>SUM(F10:F28)</f>
         <v>0</v>
       </c>
       <c r="G29" s="44">
-        <f>SUM(G9:G28)</f>
+        <f>SUM(G10:G28)</f>
         <v>0</v>
       </c>
       <c r="H29" s="44">
-        <f>SUM(H9:H28)</f>
-        <v>3000000</v>
+        <f>SUM(H10:H28)</f>
+        <v>0</v>
       </c>
       <c r="I29" s="44"/>
     </row>
@@ -9390,10 +9413,10 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="K2" s="166" t="s">
+      <c r="K2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="168"/>
+      <c r="L2" s="165"/>
       <c r="M2" s="3"/>
       <c r="N2" s="4" t="s">
         <v>10</v>
@@ -9412,10 +9435,10 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="K3" s="166" t="s">
+      <c r="K3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="168"/>
+      <c r="L3" s="165"/>
       <c r="M3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
@@ -9431,10 +9454,10 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="K4" s="172" t="s">
+      <c r="K4" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="173"/>
+      <c r="L4" s="170"/>
       <c r="M4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -9450,10 +9473,10 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="K5" s="177" t="s">
+      <c r="K5" s="174" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="178"/>
+      <c r="L5" s="175"/>
       <c r="M5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -9861,10 +9884,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="166" t="s">
+      <c r="H2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="168"/>
+      <c r="I2" s="165"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -9880,10 +9903,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="166" t="s">
+      <c r="H3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="168"/>
+      <c r="I3" s="165"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -9896,10 +9919,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="172" t="s">
+      <c r="H4" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="173"/>
+      <c r="I4" s="170"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -9912,10 +9935,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="177" t="s">
+      <c r="H5" s="174" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="178"/>
+      <c r="I5" s="175"/>
       <c r="J5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -10466,10 +10489,10 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="J2" s="166" t="s">
+      <c r="J2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="168"/>
+      <c r="K2" s="165"/>
       <c r="L2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -10484,10 +10507,10 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="J3" s="166" t="s">
+      <c r="J3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="168"/>
+      <c r="K3" s="165"/>
       <c r="L3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -10502,10 +10525,10 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="J4" s="172" t="s">
+      <c r="J4" s="169" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="173"/>
+      <c r="K4" s="170"/>
       <c r="L4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -10520,10 +10543,10 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="J5" s="177" t="s">
+      <c r="J5" s="174" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="178"/>
+      <c r="K5" s="175"/>
       <c r="L5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -10895,10 +10918,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="166" t="s">
+      <c r="H2" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="168"/>
+      <c r="I2" s="165"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -10911,10 +10934,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="166" t="s">
+      <c r="H3" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="168"/>
+      <c r="I3" s="165"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -10927,10 +10950,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="H4" s="177" t="s">
+      <c r="H4" s="174" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="178"/>
+      <c r="I4" s="175"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -10943,10 +10966,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="172" t="s">
+      <c r="H5" s="169" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="173"/>
+      <c r="I5" s="170"/>
       <c r="J5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -11313,10 +11336,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="179" t="s">
+      <c r="K2" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="180"/>
+      <c r="L2" s="177"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -11406,10 +11429,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="148" t="s">
+      <c r="H2" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="149"/>
+      <c r="I2" s="146"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -11422,10 +11445,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="179" t="s">
+      <c r="H3" s="176" t="s">
         <v>165</v>
       </c>
-      <c r="I3" s="180"/>
+      <c r="I3" s="177"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -11804,10 +11827,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="148" t="s">
+      <c r="H2" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="149"/>
+      <c r="I2" s="146"/>
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -11819,10 +11842,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="179" t="s">
+      <c r="H3" s="176" t="s">
         <v>175</v>
       </c>
-      <c r="I3" s="180"/>
+      <c r="I3" s="177"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -11836,20 +11859,20 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="27" x14ac:dyDescent="0.25">
-      <c r="B5" s="182" t="s">
+      <c r="B5" s="179" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="182"/>
-      <c r="D5" s="182"/>
-      <c r="E5" s="182"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
     </row>
     <row r="6" spans="1:14" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="183" t="s">
+      <c r="A6" s="180" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="183"/>
-      <c r="C6" s="183"/>
-      <c r="D6" s="183"/>
+      <c r="B6" s="180"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="180"/>
       <c r="E6" s="72"/>
       <c r="F6" s="72"/>
       <c r="G6" s="72"/>
@@ -11895,11 +11918,11 @@
       <c r="J9"/>
     </row>
     <row r="10" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="181" t="s">
+      <c r="B10" s="178" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="181"/>
-      <c r="D10" s="181"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="178"/>
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="71"/>
@@ -12048,11 +12071,11 @@
       <c r="J20" s="72"/>
     </row>
     <row r="21" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="181" t="s">
+      <c r="B21" s="178" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="181"/>
-      <c r="D21" s="181"/>
+      <c r="C21" s="178"/>
+      <c r="D21" s="178"/>
       <c r="E21" s="72"/>
       <c r="F21" s="72"/>
       <c r="G21" s="72"/>
@@ -12094,20 +12117,20 @@
       <c r="J24" s="68"/>
     </row>
     <row r="25" spans="1:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="B25" s="182" t="s">
+      <c r="B25" s="179" t="s">
         <v>199</v>
       </c>
-      <c r="C25" s="182"/>
-      <c r="D25" s="182"/>
-      <c r="E25" s="182"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="179"/>
+      <c r="E25" s="179"/>
     </row>
     <row r="26" spans="1:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="A26" s="183" t="s">
+      <c r="A26" s="180" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="183"/>
-      <c r="C26" s="183"/>
-      <c r="D26" s="183"/>
+      <c r="B26" s="180"/>
+      <c r="C26" s="180"/>
+      <c r="D26" s="180"/>
     </row>
     <row r="27" spans="1:10" ht="27" x14ac:dyDescent="0.25">
       <c r="B27"/>
@@ -12131,11 +12154,11 @@
       <c r="D29"/>
     </row>
     <row r="30" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="181" t="s">
+      <c r="B30" s="178" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="181"/>
-      <c r="D30" s="181"/>
+      <c r="C30" s="178"/>
+      <c r="D30" s="178"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:10" ht="27" x14ac:dyDescent="0.55000000000000004">
@@ -12229,11 +12252,11 @@
       <c r="D40" s="72"/>
     </row>
     <row r="41" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="181" t="s">
+      <c r="B41" s="178" t="s">
         <v>188</v>
       </c>
-      <c r="C41" s="181"/>
-      <c r="D41" s="181"/>
+      <c r="C41" s="178"/>
+      <c r="D41" s="178"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -12296,10 +12319,10 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="G2" s="148" t="s">
+      <c r="G2" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="149"/>
+      <c r="H2" s="146"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4" t="s">
         <v>10</v>
@@ -12314,10 +12337,10 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="G3" s="179" t="s">
+      <c r="G3" s="176" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="180"/>
+      <c r="H3" s="177"/>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -13198,9 +13221,9 @@
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13240,10 +13263,10 @@
       <c r="M1" s="126"/>
     </row>
     <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="135" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="129" t="s">
@@ -13256,11 +13279,11 @@
       </c>
       <c r="G2" s="133"/>
       <c r="H2" s="134"/>
-      <c r="I2" s="135" t="s">
+      <c r="I2" s="181" t="s">
         <v>269</v>
       </c>
-      <c r="J2" s="136"/>
-      <c r="K2" s="137"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="183"/>
       <c r="L2" s="124" t="s">
         <v>22</v>
       </c>
@@ -13269,8 +13292,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="141"/>
-      <c r="B3" s="139"/>
+      <c r="A3" s="138"/>
+      <c r="B3" s="136"/>
       <c r="C3" s="91" t="s">
         <v>270</v>
       </c>
@@ -13381,7 +13404,7 @@
         <v>15500000</v>
       </c>
       <c r="K6" s="84">
-        <f t="shared" ref="K6:K29" si="1">(K5+I6)-J6</f>
+        <f t="shared" ref="K6:K30" si="1">(K5+I6)-J6</f>
         <v>-18500000</v>
       </c>
       <c r="L6" s="85" t="s">
@@ -14093,8 +14116,13 @@
         <v>1863000</v>
       </c>
       <c r="I30" s="84"/>
-      <c r="J30" s="84"/>
-      <c r="K30" s="84"/>
+      <c r="J30" s="84">
+        <v>4899000</v>
+      </c>
+      <c r="K30" s="84">
+        <f t="shared" si="1"/>
+        <v>-21731000</v>
+      </c>
       <c r="L30" s="85" t="s">
         <v>266</v>
       </c>
@@ -14156,7 +14184,9 @@
       <c r="A33" s="39">
         <v>30</v>
       </c>
-      <c r="B33" s="85"/>
+      <c r="B33" s="85" t="s">
+        <v>309</v>
+      </c>
       <c r="C33" s="82"/>
       <c r="D33" s="82"/>
       <c r="E33" s="82"/>
@@ -14404,6 +14434,7 @@
   <hyperlinks>
     <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{C9A86160-01A7-4FFF-AE85-83614874BA51}"/>
     <hyperlink ref="F2:H2" location="'N.35 تنخواه پیمانکاری دیوارکشی'!A1" display="تنخواه دیوارکشی آقای سعیدی" xr:uid="{1B951EA9-90AF-4C68-B11E-FE74F818619A}"/>
+    <hyperlink ref="I2:K2" location="'N.34 علی الحساب موقت'!A1" display="تنخواه علی الحساب آقای جعفری" xr:uid="{BA773F72-4537-40EA-B8BF-19F26EF594A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14437,10 +14468,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="143"/>
+      <c r="B1" s="140"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -14453,10 +14484,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="144" t="s">
+      <c r="H2" s="141" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="145"/>
+      <c r="I2" s="142"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -14469,10 +14500,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="146" t="s">
+      <c r="H3" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="147"/>
+      <c r="I3" s="144"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -16937,11 +16968,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A33:E33"/>
     <mergeCell ref="A57:F57"/>
     <mergeCell ref="A204:F204"/>
     <mergeCell ref="A179:E179"/>
@@ -16949,6 +16975,11 @@
     <mergeCell ref="A82:D82"/>
     <mergeCell ref="A106:G106"/>
     <mergeCell ref="A130:H130"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A33:E33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{9E228265-015F-4ED7-804E-491796425E13}"/>
@@ -16982,16 +17013,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="143"/>
+      <c r="B1" s="140"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="148" t="s">
+      <c r="J2" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="149"/>
+      <c r="K2" s="146"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -17031,10 +17062,10 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="148" t="s">
+      <c r="J12" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="149"/>
+      <c r="K12" s="146"/>
     </row>
     <row r="13" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="2">
@@ -17105,7 +17136,7 @@
       </c>
     </row>
     <row r="24" spans="9:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="150" t="s">
+      <c r="I24" s="147" t="s">
         <v>76</v>
       </c>
       <c r="J24" s="2">
@@ -17116,7 +17147,7 @@
       </c>
     </row>
     <row r="25" spans="9:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I25" s="151"/>
+      <c r="I25" s="148"/>
       <c r="J25" s="2" t="s">
         <v>74</v>
       </c>
@@ -17147,9 +17178,7 @@
   </sheetPr>
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
+    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17168,10 +17197,10 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="152" t="s">
+      <c r="K2" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="153"/>
+      <c r="L2" s="150"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -17228,7 +17257,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -17261,10 +17290,10 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="H2" s="154" t="s">
+      <c r="H2" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="155"/>
+      <c r="I2" s="152"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4" t="s">
         <v>10</v>
@@ -17280,10 +17309,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="H3" s="156" t="s">
+      <c r="H3" s="153" t="s">
         <v>291</v>
       </c>
-      <c r="I3" s="157"/>
+      <c r="I3" s="154"/>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -17312,13 +17341,13 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="158" t="s">
+      <c r="A6" s="155" t="s">
         <v>301</v>
       </c>
-      <c r="B6" s="158"/>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158"/>
-      <c r="E6" s="158"/>
+      <c r="B6" s="155"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
     </row>
     <row r="7" spans="1:14" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="102" t="s">
@@ -17376,11 +17405,11 @@
         <v>#NAME?</v>
       </c>
       <c r="E10" s="114"/>
-      <c r="G10" s="159" t="s">
+      <c r="G10" s="156" t="s">
         <v>304</v>
       </c>
-      <c r="H10" s="159"/>
-      <c r="I10" s="159"/>
+      <c r="H10" s="156"/>
+      <c r="I10" s="156"/>
     </row>
     <row r="11" spans="1:14" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A11" s="111">
@@ -17532,10 +17561,10 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="160" t="s">
+      <c r="K2" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="161"/>
+      <c r="L2" s="158"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>

</xml_diff>

<commit_message>
general + n.04 + n.34
</commit_message>
<xml_diff>
--- a/1404.xlsx
+++ b/1404.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chaparsar.RRS\1404\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B74AD1-7B3B-44ED-9E10-2212CB4E1C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E5D48D-BE73-443F-B39C-5845CBF1E1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="902" firstSheet="14" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N.01 صفحه اصلی" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="409">
   <si>
     <t>اکسل مدیریتی ایستگاه تحقیقات برنج شهید شیرودی تنکابن سال 1404</t>
   </si>
@@ -1296,6 +1296,9 @@
   </si>
   <si>
     <t>اصلاحیه</t>
+  </si>
+  <si>
+    <t>1404/02/28</t>
   </si>
 </sst>
 </file>
@@ -8583,12 +8586,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:E62"/>
     <mergeCell ref="F62:G62"/>
     <mergeCell ref="H62:I62"/>
     <mergeCell ref="B60:C60"/>
@@ -8597,6 +8594,12 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D62:E62"/>
   </mergeCells>
   <conditionalFormatting sqref="B63:B72 D63:D72 F63:F72 H63:H72">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -9184,13 +9187,14 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="8" width="25.140625" style="1" customWidth="1"/>
@@ -9200,11 +9204,13 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+    <row r="1" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="171"/>
+      <c r="B1" s="96" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="2" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G2" s="203" t="s">
@@ -9376,17 +9382,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G6" location="'زونکن سه - تنخواه - فرم پذیرایی'!A1" display="پذیرایی" xr:uid="{5C653D19-6D92-4430-8ECC-7F774116C6F7}"/>
     <hyperlink ref="G10" location="'خلاصه وضعیت'!A1" display="خلاصه وضعیت" xr:uid="{03320E24-0EE2-4F2B-AE6E-758779E3CC2D}"/>
     <hyperlink ref="H6" location="'زونکن سه - بایگانی - پذیرایی'!A1" display="بایگانی پذیرایی" xr:uid="{CB1E63FB-A118-4DE7-8A0A-D7470D837B94}"/>
-    <hyperlink ref="I6" location="'علی الحساب موقت'!A1" display="علی الحساب موقت" xr:uid="{5FAAFCE6-9255-4966-9EE3-3ECEB1E0879E}"/>
+    <hyperlink ref="I6" location="'N.34 علی الحساب موقت'!A1" display="علی الحساب موقت" xr:uid="{5FAAFCE6-9255-4966-9EE3-3ECEB1E0879E}"/>
     <hyperlink ref="G12" location="'دفتر تنخواه'!A1" display="دفتر تنخواه" xr:uid="{E059DBBE-3FE6-4514-A094-F7E6FCE9835E}"/>
     <hyperlink ref="I7" location="'سایر فاکتورهای پرداخت شده'!A1" display="سایر فاکتورهای پرداخت شده" xr:uid="{1737F1B5-DFE8-4002-82EB-C44F71AB905A}"/>
     <hyperlink ref="G7" location="'زونکن سه - تنخواه - سوخت'!A1" display="سوخت" xr:uid="{CA289039-73A6-4D59-B9A7-CA4A67E995FC}"/>
@@ -9396,7 +9401,8 @@
     <hyperlink ref="J7" location="'لیست کارگری دیوارکشیN.33'!A1" display="لیست کارگری دیوارکشی" xr:uid="{53206997-9BBF-4503-9D4C-FCB0240C1499}"/>
     <hyperlink ref="J8" location="'لیست مصالح دیوارکشیN.32'!A1" display="لیست مصالح دیوارکشی" xr:uid="{7BCB0872-1E5C-415F-9F83-433D278358AF}"/>
     <hyperlink ref="I8" location="'خرید کود باغ مرکبات'!A1" display="خرید کود باغ مرکبات" xr:uid="{8A27CE52-3082-4A16-97D2-191C7523B1E2}"/>
-    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{B6407D15-524F-4FB2-9698-FB15B890A558}"/>
+    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{FDECAAFA-763A-44FD-80FD-39D3A615F60F}"/>
+    <hyperlink ref="B1" location="'N.04 دفتر روزانه'!A1" display="دفتر روزانه" xr:uid="{65962533-F949-43E3-AF22-588FFBB9734B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9409,8 +9415,8 @@
   </sheetPr>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K3"/>
+    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -9428,12 +9434,14 @@
     <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A1" s="7"/>
+      <c r="B1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="7"/>
+      <c r="C1" s="96" t="s">
+        <v>238</v>
+      </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -9849,16 +9857,16 @@
       <c r="N25" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H2:I2" location="'مدیریت زونکن دو'!A1" display="زونکن شماره دو" xr:uid="{B3AD33A5-7D52-4F52-AD20-8ABB5FD45AB6}"/>
-    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{4B03EBA6-9646-4E80-8A6B-10B65B506C93}"/>
+    <hyperlink ref="B1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{54521BBF-CA41-4009-B6C2-FF02742E1E4B}"/>
+    <hyperlink ref="C1" location="'N.04 دفتر روزانه'!A1" display="دفتر روزانه" xr:uid="{7696526B-92B0-4B7F-A444-11A7DB1E7750}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9873,7 +9881,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -9892,12 +9900,14 @@
     <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A1" s="7"/>
+      <c r="B1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="7"/>
+      <c r="C1" s="96" t="s">
+        <v>238</v>
+      </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -10400,8 +10410,7 @@
       <c r="F28" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="5">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
@@ -10411,7 +10420,8 @@
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I2:J2" location="'N3 زونکن سه'!A1" display="زونکن شماره سه" xr:uid="{B0FD323F-2076-4EAB-A5C0-74D9B40EE584}"/>
-    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{BF48CFC8-656B-4342-809D-12DD43CE1D68}"/>
+    <hyperlink ref="B1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{E18FA9FF-A479-4BFD-AAF9-022F58429D7B}"/>
+    <hyperlink ref="C1" location="'N.04 دفتر روزانه'!A1" display="دفتر روزانه" xr:uid="{C487D282-5421-4A4E-8F0E-3D099DB1FB66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10595,8 +10605,8 @@
   </sheetPr>
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" rightToLeft="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -10619,12 +10629,14 @@
     <col min="16" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A1" s="7"/>
+      <c r="B1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="7"/>
+      <c r="C1" s="96" t="s">
+        <v>238</v>
+      </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -11475,8 +11487,7 @@
       <c r="F29" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="9">
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="M7:O7"/>
@@ -11490,7 +11501,8 @@
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J2:K2" location="'N3 زونکن سه'!A1" display="زونکن شماره سه" xr:uid="{222970F7-877D-4191-B67C-78F0AA6BFC47}"/>
-    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{2F7EC349-6EB5-4394-A4D0-FF3EBEF8A8AD}"/>
+    <hyperlink ref="B1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{31D82A48-68FF-4EE9-9FC7-393EA2E04DDD}"/>
+    <hyperlink ref="C1" location="'N.04 دفتر روزانه'!A1" display="دفتر روزانه" xr:uid="{0DE6BB38-06F6-4002-A3C1-F7DD5D7923ED}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="66" orientation="landscape" r:id="rId1"/>
@@ -11504,9 +11516,7 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L3"/>
-    </sheetView>
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11524,12 +11534,13 @@
     <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="B1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="7"/>
+      <c r="C1" s="96" t="s">
+        <v>238</v>
+      </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -11707,7 +11718,7 @@
         <v>352000</v>
       </c>
       <c r="F11" s="38">
-        <f t="shared" ref="F11:F22" si="0">(F10+D11)-E11</f>
+        <f t="shared" ref="F11:F23" si="0">(F10+D11)-E11</f>
         <v>7749000</v>
       </c>
       <c r="G11" s="8"/>
@@ -11926,11 +11937,20 @@
       <c r="A23" s="38">
         <v>15</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
+      <c r="B23" s="38" t="s">
+        <v>408</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>135</v>
+      </c>
       <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
+      <c r="E23" s="38">
+        <v>321000</v>
+      </c>
+      <c r="F23" s="38">
+        <f t="shared" si="0"/>
+        <v>7948000</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="27" x14ac:dyDescent="0.25">
       <c r="A24" s="38">
@@ -11983,17 +12003,17 @@
       <c r="F28" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2:J2" location="'زونکن سه - تنخواه'!A1" display="زونکن شماره سه" xr:uid="{CD3FC5BE-D291-4EE9-BD24-4A249B0FBE7C}"/>
-    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{56019AFD-8239-4232-BC40-87A8C315A85E}"/>
+    <hyperlink ref="I2:J2" location="'N3 زونکن سه'!A1" display="زونکن شماره سه" xr:uid="{CD3FC5BE-D291-4EE9-BD24-4A249B0FBE7C}"/>
+    <hyperlink ref="B1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{8FB3D715-4FE2-45B3-89B0-F09EB2C8AF76}"/>
+    <hyperlink ref="C1" location="'N.04 دفتر روزانه'!A1" display="دفتر روزانه" xr:uid="{5489275A-827E-4B91-B187-4CD032CEEFF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12536,7 +12556,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K3"/>
+      <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -12554,11 +12574,9 @@
     <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="171"/>
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -12750,16 +12768,14 @@
       <c r="I16" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H2:I2" location="'زونکن سه - تنخواه'!A1" display="زونکن شماره سه" xr:uid="{FC3DEBD9-C77E-418F-928F-295C349969DF}"/>
-    <hyperlink ref="A1" location="'N.01 صفحه اصلی'!A1" display="صفحه اصلی" xr:uid="{66B279A8-FAAD-49ED-98C3-48C47A08E71B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18179,8 +18195,8 @@
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
@@ -18360,7 +18376,7 @@
         <v>15500000</v>
       </c>
       <c r="K6" s="80">
-        <f t="shared" ref="K6:K34" si="1">(K5+I6)-J6</f>
+        <f t="shared" ref="K6:K41" si="1">(K5+I6)-J6</f>
         <v>-18500000</v>
       </c>
       <c r="L6" s="81" t="s">
@@ -19209,7 +19225,10 @@
       </c>
       <c r="I35" s="80"/>
       <c r="J35" s="80"/>
-      <c r="K35" s="80"/>
+      <c r="K35" s="80">
+        <f t="shared" si="1"/>
+        <v>8269000</v>
+      </c>
       <c r="L35" s="38" t="s">
         <v>311</v>
       </c>
@@ -19235,7 +19254,10 @@
       </c>
       <c r="I36" s="80"/>
       <c r="J36" s="80"/>
-      <c r="K36" s="80"/>
+      <c r="K36" s="80">
+        <f t="shared" si="1"/>
+        <v>8269000</v>
+      </c>
       <c r="L36" s="81" t="s">
         <v>319</v>
       </c>
@@ -19261,7 +19283,10 @@
       </c>
       <c r="I37" s="80"/>
       <c r="J37" s="80"/>
-      <c r="K37" s="80"/>
+      <c r="K37" s="80">
+        <f t="shared" si="1"/>
+        <v>8269000</v>
+      </c>
       <c r="L37" s="81" t="s">
         <v>128</v>
       </c>
@@ -19289,7 +19314,10 @@
       </c>
       <c r="I38" s="80"/>
       <c r="J38" s="80"/>
-      <c r="K38" s="80"/>
+      <c r="K38" s="80">
+        <f t="shared" si="1"/>
+        <v>8269000</v>
+      </c>
       <c r="L38" s="38" t="s">
         <v>321</v>
       </c>
@@ -19315,7 +19343,10 @@
       </c>
       <c r="I39" s="80"/>
       <c r="J39" s="80"/>
-      <c r="K39" s="80"/>
+      <c r="K39" s="80">
+        <f t="shared" si="1"/>
+        <v>8269000</v>
+      </c>
       <c r="L39" s="81" t="s">
         <v>323</v>
       </c>
@@ -19341,7 +19372,10 @@
       </c>
       <c r="I40" s="80"/>
       <c r="J40" s="80"/>
-      <c r="K40" s="80"/>
+      <c r="K40" s="80">
+        <f t="shared" si="1"/>
+        <v>8269000</v>
+      </c>
       <c r="L40" s="81" t="s">
         <v>263</v>
       </c>
@@ -19351,7 +19385,9 @@
       <c r="A41" s="38">
         <v>38</v>
       </c>
-      <c r="B41" s="81"/>
+      <c r="B41" s="81" t="s">
+        <v>408</v>
+      </c>
       <c r="C41" s="78"/>
       <c r="D41" s="78"/>
       <c r="E41" s="78"/>
@@ -19359,8 +19395,13 @@
       <c r="G41" s="79"/>
       <c r="H41" s="79"/>
       <c r="I41" s="80"/>
-      <c r="J41" s="80"/>
-      <c r="K41" s="80"/>
+      <c r="J41" s="80">
+        <v>321000</v>
+      </c>
+      <c r="K41" s="80">
+        <f t="shared" si="1"/>
+        <v>7948000</v>
+      </c>
       <c r="L41" s="81"/>
       <c r="M41" s="81"/>
     </row>

</xml_diff>